<commit_message>
PROS 5151 - MARSRU TEMPLATE UPDATE
</commit_message>
<xml_diff>
--- a/Projects/MARSRU_PROD/Data/MARS must-range targets.xlsx
+++ b/Projects/MARSRU_PROD/Data/MARS must-range targets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="1648" sheetId="1" state="visible" r:id="rId2"/>
@@ -34,28 +34,28 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="98">
   <si>
-    <t>Store type</t>
-  </si>
-  <si>
-    <t>Region</t>
-  </si>
-  <si>
-    <t>EAN</t>
-  </si>
-  <si>
-    <t>Grocery Магазин у дома (&lt;100),
+    <t xml:space="preserve">Store type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Region</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grocery Магазин у дома (&lt;100),
 Grocery Магазин у дома (100-299),
 Grocery Магазин у дома (300-449),
 Grocery Магазин у дома (450-599),
 Grocery Магазин у дома (600-999)</t>
   </si>
   <si>
-    <t>1-ый Food,
+    <t xml:space="preserve">1-ый Food,
 1-ый Gr,
 1-ый ZOO</t>
   </si>
   <si>
-    <t>4607065003999,
+    <t xml:space="preserve">4607065003999,
 4607065004019,
 4607065004057,
 4607065004118,
@@ -87,14 +87,14 @@
 5000159450881</t>
   </si>
   <si>
-    <t>1+2 кластер,
+    <t xml:space="preserve">1+2 кластер,
 2-ой Food,
 2-ой Gr,
 2-ой ZOO
 </t>
   </si>
   <si>
-    <t>4607065003999,
+    <t xml:space="preserve">4607065003999,
 4607065004019,
 4607065004057,
 4607065004118,
@@ -127,14 +127,14 @@
 </t>
   </si>
   <si>
-    <t>3+4 кластер,
+    <t xml:space="preserve">3+4 кластер,
 3-ий Food,
 3-ий Gr,
 3-ий ZOO
 </t>
   </si>
   <si>
-    <t>4607065003999,
+    <t xml:space="preserve">4607065003999,
 4607065004019,
 4607065004057,
 4607065004118,
@@ -167,11 +167,11 @@
 </t>
   </si>
   <si>
-    <t>Grocery Дискаунтер (&lt;300),
+    <t xml:space="preserve">Grocery Дискаунтер (&lt;300),
 Grocery Дискаунтер (300-999)</t>
   </si>
   <si>
-    <t>4607065003999,
+    <t xml:space="preserve">4607065003999,
 4607065004019,
 4607065004057,
 4607065004118,
@@ -203,7 +203,7 @@
 5000159450881</t>
   </si>
   <si>
-    <t>1+2 кластер,
+    <t xml:space="preserve">1+2 кластер,
 2-ой Food,
 2-ой Gr
 2-ой ZOO,
@@ -213,7 +213,7 @@
 3-ий ZOO</t>
   </si>
   <si>
-    <t>4607065003999,
+    <t xml:space="preserve">4607065003999,
 4607065004019,
 4607065004057,
 4607065004118,
@@ -246,11 +246,11 @@
 </t>
   </si>
   <si>
-    <t>Grocery BIG BOXES (1000-2499),
+    <t xml:space="preserve">Grocery BIG BOXES (1000-2499),
 Grocery BIG BOXES (2500+)</t>
   </si>
   <si>
-    <t>4607065003999,
+    <t xml:space="preserve">4607065003999,
 4607065004019,
 4607065004057,
 4607065004118,
@@ -282,7 +282,7 @@
 5000159450881</t>
   </si>
   <si>
-    <t>4607065003999,
+    <t xml:space="preserve">4607065003999,
 4607065004019,
 4607065004057,
 4607065004118,
@@ -315,7 +315,7 @@
 </t>
   </si>
   <si>
-    <t>SPT Киоск,
+    <t xml:space="preserve">SPT Киоск,
 SPT За прилавком (&lt; 20 м2),
 SPT За прилавком (&gt;= 20 м2),
 SPT Самообслуживание (&lt; 20 м2),
@@ -324,7 +324,7 @@
 SPT Самообслуживание (&gt;= 100 м2)</t>
   </si>
   <si>
-    <t>4607065003999,
+    <t xml:space="preserve">4607065003999,
 4607065004019,
 5000159438940,
 4607065004118,
@@ -356,25 +356,25 @@
 4607065003135</t>
   </si>
   <si>
-    <t>5998749123072/4607065001063, 5998749123058/4607065001025</t>
-  </si>
-  <si>
-    <t>5998749123072/4607065001063, 5998749123058/4607065001025, 5998749123065/4607065001049</t>
-  </si>
-  <si>
-    <t>5998749106877, 5998749104392</t>
-  </si>
-  <si>
-    <t>5998749106877, 5998749104392, 5998749108147</t>
-  </si>
-  <si>
-    <t>SPT Самообслуживание (&lt; 20 м2)
+    <t xml:space="preserve">5998749123072/4607065001063, 5998749123058/4607065001025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5998749123072/4607065001063, 5998749123058/4607065001025, 5998749123065/4607065001049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5998749106877, 5998749104392</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5998749106877, 5998749104392, 5998749108147</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPT Самообслуживание (&lt; 20 м2)
 SPT Самообслуживание (&gt;= 100 м2)
 SPT Самообслуживание (20-49 м2)
 SPT Самообслуживание (50-99 м2)</t>
   </si>
   <si>
-    <t>4607065004118,
+    <t xml:space="preserve">4607065004118,
 4607065372217,
 5000159438940,
 4607065002466,
@@ -406,7 +406,7 @@
 4770608256067/4607065376475/4770608256067</t>
   </si>
   <si>
-    <t>4607065004118,
+    <t xml:space="preserve">4607065004118,
 4607065372217,
 5000159438940,
 4607065002466,
@@ -438,7 +438,7 @@
 4607065003135</t>
   </si>
   <si>
-    <t>4607065004118,
+    <t xml:space="preserve">4607065004118,
 4607065372217,
 5000159438940,
 4607065002466,
@@ -470,16 +470,16 @@
 4607065371166/5000159369688</t>
   </si>
   <si>
-    <t>4607065001063/5998749123072/4607065001025/5998749123058</t>
-  </si>
-  <si>
-    <t>4607065001063/5998749123072/4607065001025/5998749123058/5998749123065/4607065001049</t>
-  </si>
-  <si>
-    <t>5998749106877/5998749104392/5998749108147</t>
-  </si>
-  <si>
-    <t>Grocery Магазин у дома (&lt;100),
+    <t xml:space="preserve">4607065001063/5998749123072/4607065001025/5998749123058</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4607065001063/5998749123072/4607065001025/5998749123058/5998749123065/4607065001049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5998749106877/5998749104392/5998749108147</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grocery Магазин у дома (&lt;100),
 Grocery Магазин у дома (100-299),
 Grocery Магазин у дома (300-449),
 Grocery Магазин у дома (450-599),
@@ -490,22 +490,22 @@
 Grocery BIG BOXES (2500+)</t>
   </si>
   <si>
-    <t>4008429033230/4008429033278/4607065001421,
+    <t xml:space="preserve">4008429033230/4008429033278/4607065374914/4607065001421,
 4607065001612,
 5998749106877,
 4607065001063,
 5000159438735</t>
   </si>
   <si>
-    <t>4607065376048,
+    <t xml:space="preserve">4607065376048,
 4607065002862,
-4008429033230/4008429033278/4607065001421,
+4008429033230/4008429033278/4607065374914/4607065001421,
 4607065375119/4607065375188/4607065375249/4607065375317/4607065375188/4607065375119,
 5000159450881
 </t>
   </si>
   <si>
-    <t>4607065376048,
+    <t xml:space="preserve">4607065376048,
 4607065373344/4607065371241/4607065371227/4607065371265,
 4607065002862,
 4607065375119/4607065375188/4607065375249/4607065375317/4607065375188/4607065375119,
@@ -513,7 +513,7 @@
 </t>
   </si>
   <si>
-    <t>4607065003999,
+    <t xml:space="preserve">4607065003999,
 4607065004019,
 4607065004057,
 4607065004118,
@@ -540,193 +540,193 @@
 4607065002688/4607065002596/4607065371036/4607065002541</t>
   </si>
   <si>
-    <t>Shelf # from the bottom</t>
-  </si>
-  <si>
-    <t>Grocery BIG BOXES (1000-2499)</t>
-  </si>
-  <si>
-    <t>2-6</t>
-  </si>
-  <si>
-    <t>Grocery BIG BOXES (2500+)</t>
-  </si>
-  <si>
-    <t>Grocery Дискаунтер (&lt;300)</t>
-  </si>
-  <si>
-    <t>3-6</t>
-  </si>
-  <si>
-    <t>Grocery Дискаунтер (300-999)</t>
-  </si>
-  <si>
-    <t>Grocery Магазин у дома (&lt;100)</t>
-  </si>
-  <si>
-    <t>Grocery Магазин у дома (100-299)</t>
-  </si>
-  <si>
-    <t>Grocery Магазин у дома (300-449)</t>
-  </si>
-  <si>
-    <t>Grocery Магазин у дома (450-599)</t>
-  </si>
-  <si>
-    <t>Grocery Магазин у дома (600-999)</t>
-  </si>
-  <si>
-    <t>Attribute 5</t>
-  </si>
-  <si>
-    <t>Shelf length FROM INCLUDING</t>
-  </si>
-  <si>
-    <t>Shelf length TO EXCLUDING</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>Comment 2</t>
-  </si>
-  <si>
-    <t>Comment 3</t>
-  </si>
-  <si>
-    <t>1-ый Gr</t>
-  </si>
-  <si>
-    <t>ANY</t>
-  </si>
-  <si>
-    <t>1 кл. 1,6м Дискаунтер</t>
-  </si>
-  <si>
-    <t>&gt;=1,6</t>
-  </si>
-  <si>
-    <t>(2261/2264)+(2265/2351)</t>
-  </si>
-  <si>
-    <t>1 кл. 1,6м Маг. у дома</t>
-  </si>
-  <si>
-    <t>&gt;=1,6&lt;2,4</t>
-  </si>
-  <si>
-    <t>1 кл. 2,4м Маг. у дома</t>
-  </si>
-  <si>
-    <t>&gt;=2,4</t>
-  </si>
-  <si>
-    <t>&gt;=2.4&lt;3</t>
-  </si>
-  <si>
-    <t>1 кл. 3м Маг. у дома</t>
-  </si>
-  <si>
-    <t>&gt;=3</t>
-  </si>
-  <si>
-    <t>&gt;=3&lt;4</t>
-  </si>
-  <si>
-    <t>1 кл. 4м Маг. у дома</t>
-  </si>
-  <si>
-    <t>&gt;=4&lt;5</t>
-  </si>
-  <si>
-    <t>&gt;=4</t>
-  </si>
-  <si>
-    <t>1 кл. 5м Гипермаркет</t>
-  </si>
-  <si>
-    <t>&gt;=5</t>
-  </si>
-  <si>
-    <t>&gt;=5&lt;7</t>
-  </si>
-  <si>
-    <t>1 кл. 6м (линейн) Дискаунтер</t>
-  </si>
-  <si>
-    <t>любое</t>
-  </si>
-  <si>
-    <t>&gt;0&lt;1,6</t>
-  </si>
-  <si>
-    <t>1 кл. 6м (линейн) Маг. у дома</t>
-  </si>
-  <si>
-    <t>1 кл. 7м Гипермаркет</t>
-  </si>
-  <si>
-    <t>&gt;=7</t>
-  </si>
-  <si>
-    <t>1 кл.1,6 м Маг. у дома</t>
-  </si>
-  <si>
-    <t>1 кл.2,4м Маг. у дома</t>
-  </si>
-  <si>
-    <t>&gt;=2,4&lt;3</t>
-  </si>
-  <si>
-    <t>2-ой Gr</t>
-  </si>
-  <si>
-    <t>2 кл. 6м (линейн) Дискаунтер</t>
-  </si>
-  <si>
-    <t>2 кл. 6м (линейн) Маг. у дома</t>
-  </si>
-  <si>
-    <t>3-ий Gr</t>
-  </si>
-  <si>
-    <t>2-3 кл. 1,6 м  Маг. у дома</t>
-  </si>
-  <si>
-    <t>2-3 кл. 1,6 м Маг. у дома</t>
-  </si>
-  <si>
-    <t>2-3 кл. 1,6м Дискаунтер</t>
-  </si>
-  <si>
-    <t>2-3 кл. 1,6м Маг. у дома</t>
-  </si>
-  <si>
-    <t>2-3 кл. 2,4 м Маг. у дома</t>
-  </si>
-  <si>
-    <t>2-3 кл. 2,4м Маг. у дома</t>
-  </si>
-  <si>
-    <t>2-3 кл. 3м Маг. у дома</t>
-  </si>
-  <si>
-    <t>2-3 кл. 4м Маг. у дома</t>
-  </si>
-  <si>
-    <t>2-3 кл. 5м Гипермаркет</t>
-  </si>
-  <si>
-    <t>2-3 кл. 7м Гипермаркет</t>
-  </si>
-  <si>
-    <t>3 кл. 6м (линейн) Дискаунтер</t>
-  </si>
-  <si>
-    <t>3 кл. 6м (линейн) Маг. у дома</t>
+    <t xml:space="preserve">Shelf # from the bottom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grocery BIG BOXES (1000-2499)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grocery BIG BOXES (2500+)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grocery Дискаунтер (&lt;300)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grocery Дискаунтер (300-999)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grocery Магазин у дома (&lt;100)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grocery Магазин у дома (100-299)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grocery Магазин у дома (300-449)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grocery Магазин у дома (450-599)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grocery Магазин у дома (600-999)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attribute 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shelf length FROM INCLUDING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shelf length TO EXCLUDING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-ый Gr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 кл. 1,6м Дискаунтер</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;=1,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(2261/2264)+(2265/2351)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 кл. 1,6м Маг. у дома</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;=1,6&lt;2,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 кл. 2,4м Маг. у дома</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;=2,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;=2.4&lt;3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 кл. 3м Маг. у дома</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;=3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;=3&lt;4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 кл. 4м Маг. у дома</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;=4&lt;5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 кл. 5м Гипермаркет</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;=5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;=5&lt;7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 кл. 6м (линейн) Дискаунтер</t>
+  </si>
+  <si>
+    <t xml:space="preserve">любое</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;0&lt;1,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 кл. 6м (линейн) Маг. у дома</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 кл. 7м Гипермаркет</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;=7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 кл.1,6 м Маг. у дома</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 кл.2,4м Маг. у дома</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;=2,4&lt;3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-ой Gr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 кл. 6м (линейн) Дискаунтер</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 кл. 6м (линейн) Маг. у дома</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-ий Gr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-3 кл. 1,6 м  Маг. у дома</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-3 кл. 1,6 м Маг. у дома</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-3 кл. 1,6м Дискаунтер</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-3 кл. 1,6м Маг. у дома</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-3 кл. 2,4 м Маг. у дома</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-3 кл. 2,4м Маг. у дома</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-3 кл. 3м Маг. у дома</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-3 кл. 4м Маг. у дома</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-3 кл. 5м Гипермаркет</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-3 кл. 7м Гипермаркет</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 кл. 6м (линейн) Дискаунтер</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 кл. 6м (линейн) Маг. у дома</t>
   </si>
 </sst>
 </file>
@@ -734,7 +734,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
@@ -993,10 +993,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.4534412955466"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.7732793522267"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.5425101214575"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.9068825910931"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.0323886639676"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.81376518218623"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1105,16 +1105,16 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.9919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="59.0242914979757"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="78.3036437246964"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.0323886639676"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.4777327935223"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="80.1902834008097"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.30364372469636"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1128,7 +1128,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="117.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
         <v>30</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="117.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
         <v>30</v>
       </c>
@@ -1185,10 +1185,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.5263157894737"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.0607287449393"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.8137651821862"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.6477732793522"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.251012145749"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.8056680161943"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.30364372469636"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1259,9 +1259,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.8056680161943"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.81376518218623"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1362,22 +1362,22 @@
   </sheetPr>
   <dimension ref="A1:I94"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A69" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A69" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C82" activeCellId="0" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.2429149797571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="27.2064777327935"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.31983805668016"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.2753036437247"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.0323886639676"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.4251012145749"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.0607287449393"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.1133603238866"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="27.9068825910931"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.7732793522267"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.48987854251012"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.2550607287449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.3805668016194"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.9716599190283"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.30364372469636"/>
   </cols>
   <sheetData>
     <row r="1" s="13" customFormat="true" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3849,10 +3849,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.5951417004049"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.2388663967611"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.5991902834008"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.1093117408907"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.6275303643725"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.81376518218623"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3923,10 +3923,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.5951417004049"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.2388663967611"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.8016194331984"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.1093117408907"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.6518218623482"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.81376518218623"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3997,10 +3997,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.5951417004049"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.2388663967611"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="72.7327935222672"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.1093117408907"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.5546558704453"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.81376518218623"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4071,9 +4071,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="37.17004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="163.570850202429"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="5" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="37.9473684210526"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="167.720647773279"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="5" width="9.30364372469636"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4132,9 +4132,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="47.7732793522267"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="32.0283400809717"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="5" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="48.8461538461539"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="32.8056680161943"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="5" width="9.30364372469636"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4193,10 +4193,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="59.4493927125506"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.0931174089069"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.2388663967611"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.9635627530364"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.4574898785425"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.2348178137652"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.81376518218623"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4267,9 +4267,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="37.7044534412955"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="146.858299595142"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="5" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="38.6842105263158"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="150.578947368421"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="5" width="9.30364372469636"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4328,9 +4328,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="48.6315789473684"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="74.9838056680162"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="5" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="49.8259109311741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="76.8825910931174"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="5" width="9.30364372469636"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
PROS 5150 - MARSRU TEMPLATE UPDATE (kpi 2390)
</commit_message>
<xml_diff>
--- a/Projects/MARSRU_PROD/Data/MARS must-range targets.xlsx
+++ b/Projects/MARSRU_PROD/Data/MARS must-range targets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="1648" sheetId="1" state="visible" r:id="rId2"/>
@@ -528,7 +528,7 @@
 4607065375829,
 5000159438674,
 4607065374877/4607065375164/4607065375225/4607065375300/4607065375164/4607065374877/4607065730932,
-4607065375034,
+4607065375034/5000159451802/4607065003098,
 4607065378424,
 4011100158399/5000159441766/5000159380850/5000159425513,
 5000159438926,
@@ -993,10 +993,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.5425101214575"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.9068825910931"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.0323886639676"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.81376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.3967611336032"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="59.251012145749"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.251012145749"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.06072874493927"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1105,16 +1105,16 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.0323886639676"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.4777327935223"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="80.1902834008097"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.30364372469636"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.1336032388664"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.9433198380567"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="82.2672064777328"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.4251012145749"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1179,16 +1179,16 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.6477732793522"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.251012145749"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.8056680161943"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.30364372469636"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.7449392712551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="117.80971659919"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.4251012145749"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1202,7 +1202,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="417.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="321.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
         <v>30</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="417.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="321.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
         <v>30</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="417.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="321.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
         <v>30</v>
       </c>
@@ -1253,15 +1253,15 @@
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.8056680161943"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.81376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.663967611336"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.2995951417004"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.06072874493927"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1362,22 +1362,22 @@
   </sheetPr>
   <dimension ref="A1:I94"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A69" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A69" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C82" activeCellId="0" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.0607287449393"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.1133603238866"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="27.9068825910931"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.7732793522267"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.48987854251012"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.2550607287449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.3805668016194"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.9716599190283"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.30364372469636"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4251012145749"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.9716599190283"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="28.5222672064777"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="26.3238866396761"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.61133603238866"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="42.2348178137652"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.753036437247"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.587044534413"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.4251012145749"/>
   </cols>
   <sheetData>
     <row r="1" s="13" customFormat="true" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3849,10 +3849,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.1093117408907"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.6275303643725"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.81376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="61.5789473684211"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.9433198380567"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.06072874493927"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3923,10 +3923,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.1093117408907"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.6518218623482"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.81376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="61.5789473684211"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.9433198380567"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.6153846153846"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.06072874493927"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3997,10 +3997,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.1093117408907"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.5546558704453"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.81376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="61.5789473684211"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.9433198380567"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.06072874493927"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4071,9 +4071,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="37.9473684210526"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="167.720647773279"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="5" width="9.30364372469636"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="38.9352226720648"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="172.004048582996"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="5" width="9.4251012145749"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4132,9 +4132,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="48.8461538461539"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="32.8056680161943"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="5" width="9.30364372469636"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="50.0688259109312"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="33.5425101214575"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="5" width="9.4251012145749"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4187,16 +4187,16 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.9635627530364"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.4574898785425"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.2348178137652"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.81376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.4372469635628"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.8016194331984"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.06072874493927"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4261,15 +4261,15 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="38.6842105263158"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="150.578947368421"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="5" width="9.30364372469636"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="39.5425101214575"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="154.372469635628"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="5" width="9.4251012145749"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4322,15 +4322,15 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="49.8259109311741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="76.8825910931174"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="5" width="9.30364372469636"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="51.0445344129555"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="78.7165991902834"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="5" width="9.4251012145749"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
PROS-5305 PROS-5307 - MARSRU - Template Update
</commit_message>
<xml_diff>
--- a/Projects/MARSRU_PROD/Data/MARS must-range targets.xlsx
+++ b/Projects/MARSRU_PROD/Data/MARS must-range targets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="1648" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="108">
   <si>
     <t xml:space="preserve">Store type</t>
   </si>
@@ -470,13 +470,10 @@
 4607065371166/5000159369688</t>
   </si>
   <si>
-    <t xml:space="preserve">4607065001063/5998749123072/4607065001025/5998749123058</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4607065001063/5998749123072/4607065001025/5998749123058/5998749123065/4607065001049</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5998749106877/5998749104392/5998749108147</t>
+    <t xml:space="preserve">4607065001063/5998749123072/4607065001025/5998749123058/4607065004514/5998749106877/5998749104392</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4607065001063/5998749123072/4607065001025/5998749123058/4607065004514/4607065004446/5998749106877/5998749104392/5998749108147</t>
   </si>
   <si>
     <t xml:space="preserve">Grocery Магазин у дома (&lt;100),
@@ -490,26 +487,27 @@
 Grocery BIG BOXES (2500+)</t>
   </si>
   <si>
-    <t xml:space="preserve">4008429033230/4008429033278/4607065374914/4607065001421,
+    <t xml:space="preserve">4607065377984,
 4607065001612,
 5998749106877,
 4607065001063,
-5000159438735</t>
+5000159438735
+</t>
   </si>
   <si>
     <t xml:space="preserve">4607065376048,
 4607065002862,
-4008429033230/4008429033278/4607065374914/4607065001421,
-4607065375119/4607065375188/4607065375249/4607065375317/4607065375188/4607065375119,
+4607065377984,
+4607065375119,
 5000159450881
 </t>
   </si>
   <si>
     <t xml:space="preserve">4607065376048,
-4607065373344/4607065371241/4607065371227/4607065371265,
 4607065002862,
-4607065375119/4607065375188/4607065375249/4607065375317/4607065375188/4607065375119,
-4607065372095
+4607065002862,
+4607065375119,
+4607065004071
 </t>
   </si>
   <si>
@@ -525,19 +523,47 @@
 5000159438698,
 4011100157361,
 4607065003838,
-4607065375829,
+4607065374792,
 5000159438674,
-4607065374877/4607065375164/4607065375225/4607065375300/4607065375164/4607065374877/4607065730932,
-4607065375034/5000159451802/4607065003098,
+4607065374877,
+4607065375034,
 4607065378424,
-4011100158399/5000159441766/5000159380850/5000159425513,
+4011100158399,
 5000159438926,
 5000159438940,
-4607065371166/4607065371180/4607065371203,
+4607065371166,
 4607065372217,
 4607065372156,
 4607065003944,
-4607065002688/4607065002596/4607065371036/4607065002541</t>
+4607065002688</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4607065003999,
+4607065004019,
+4607065004057,
+4607065004118,
+4607065375966,
+4607065376000,
+4607065376062,
+4607065372057,
+5000159373111,
+5000159438698,
+4011100157361,
+4607065003838,
+4607065374792,
+5000159438674,
+4607065374877,
+4607065375034,
+4607065378424,
+4011100158399,
+5000159438926,
+5000159438940,
+4607065371166,
+4607065372217,
+4607065372156,
+4607065003944,
+4607065002688
+</t>
   </si>
   <si>
     <t xml:space="preserve">Shelf # from the bottom</t>
@@ -693,34 +719,64 @@
     <t xml:space="preserve">3-ий Gr</t>
   </si>
   <si>
-    <t xml:space="preserve">2-3 кл. 1,6 м  Маг. у дома</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-3 кл. 1,6 м Маг. у дома</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-3 кл. 1,6м Дискаунтер</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-3 кл. 1,6м Маг. у дома</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-3 кл. 2,4 м Маг. у дома</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-3 кл. 2,4м Маг. у дома</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-3 кл. 3м Маг. у дома</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-3 кл. 4м Маг. у дома</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-3 кл. 5м Гипермаркет</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-3 кл. 7м Гипермаркет</t>
+    <t xml:space="preserve">3 кл. 1,6 м  Маг. у дома</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 кл. 1,6 м Маг. у дома</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 кл. 1,6м Дискаунтер</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 кл. 1,6м Дискаунтер</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 кл. 1,6м Маг. у дома</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2  кл. 2,4 м Маг. у дома</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 кл. 2,4 м Маг. у дома</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 кл. 2,4м Маг. у дома</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 кл. 2,4м Маг. у дома</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2  кл. 2,4м Маг. у дома</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2  кл. 3м Маг. у дома</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 кл. 3м Маг. у дома</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 кл. 3м Маг. у дома</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2  кл. 4м Маг. у дома</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 кл. 4м Маг. у дома</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 кл. 5м Гипермаркет</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 кл. 5м Гипермаркет</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2  кл. 5м Гипермаркет</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 кл. 7м Гипермаркет</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 кл. 7м Гипермаркет</t>
   </si>
   <si>
     <t xml:space="preserve">3 кл. 6м (линейн) Дискаунтер</t>
@@ -733,12 +789,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -762,10 +817,17 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val=""/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val=""/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -826,7 +888,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -868,7 +930,15 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -892,18 +962,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -993,10 +1059,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.3967611336032"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="59.251012145749"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.251012145749"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.8137651821862"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="59.7732793522267"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1106,14 +1172,14 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.1336032388664"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.9433198380567"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="82.2672064777328"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.4534412955466"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.4493927125506"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="82.9109311740891"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.4251012145749"/>
   </cols>
   <sheetData>
@@ -1128,37 +1194,37 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="117.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="121.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="117.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C2" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="121.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="121.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>33</v>
+      <c r="C4" s="11" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1177,17 +1243,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.7449392712551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="117.80971659919"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.2024291497976"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.0607287449393"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="118.793522267206"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.4251012145749"/>
   </cols>
   <sheetData>
@@ -1202,20 +1268,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="321.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="356.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="321.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C2" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="350.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>6</v>
@@ -1224,9 +1290,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="321.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="350.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>8</v>
@@ -1235,6 +1301,28 @@
         <v>34</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1259,21 +1347,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.663967611336"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.2995951417004"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.9554655870445"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="13" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="14" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -1281,7 +1369,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="14" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="0" t="s">
@@ -1289,7 +1377,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="14" t="s">
         <v>39</v>
       </c>
       <c r="B4" s="0" t="s">
@@ -1297,7 +1385,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="14" t="s">
         <v>41</v>
       </c>
       <c r="B5" s="0" t="s">
@@ -1305,7 +1393,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="14" t="s">
         <v>42</v>
       </c>
       <c r="B6" s="0" t="s">
@@ -1313,7 +1401,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="14" t="s">
         <v>43</v>
       </c>
       <c r="B7" s="0" t="s">
@@ -1321,7 +1409,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="14" t="s">
         <v>44</v>
       </c>
       <c r="B8" s="0" t="s">
@@ -1329,7 +1417,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="14" t="s">
         <v>45</v>
       </c>
       <c r="B9" s="0" t="s">
@@ -1337,7 +1425,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="14" t="s">
         <v>46</v>
       </c>
       <c r="B10" s="0" t="s">
@@ -1362,2466 +1450,2466 @@
   </sheetPr>
   <dimension ref="A1:I94"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A69" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C82" activeCellId="0" sqref="C82"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4251012145749"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.9716599190283"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="28.5222672064777"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="26.3238866396761"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.61133603238866"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="42.2348178137652"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.753036437247"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.587044534413"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.6396761133603"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.2793522267206"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="15" width="28.8137651821862"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="15" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.53441295546559"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="42.5263157894737"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.4251012145749"/>
   </cols>
   <sheetData>
-    <row r="1" s="13" customFormat="true" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
+    <row r="1" s="15" customFormat="true" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="15"/>
-      <c r="G1" s="10" t="s">
+      <c r="F1" s="17"/>
+      <c r="G1" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="19" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="18" t="n">
+      <c r="C2" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="19" t="n">
+      <c r="E2" s="0" t="n">
         <v>1834</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="18" t="n">
+      <c r="C3" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="19" t="n">
+      <c r="E3" s="0" t="n">
         <v>1832</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="I3" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="16" t="n">
+      <c r="C4" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="D4" s="16" t="n">
+      <c r="D4" s="15" t="n">
         <v>2.4</v>
       </c>
-      <c r="E4" s="19" t="n">
+      <c r="E4" s="0" t="n">
         <v>1832</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="I4" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="16" t="n">
+      <c r="C5" s="15" t="n">
         <v>2.4</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="E5" s="19" t="n">
+      <c r="E5" s="0" t="n">
         <v>1836</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="I5" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="16" t="n">
+      <c r="C6" s="15" t="n">
         <v>2.4</v>
       </c>
-      <c r="D6" s="16" t="n">
+      <c r="D6" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="E6" s="19" t="n">
+      <c r="E6" s="0" t="n">
         <v>1836</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="H6" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="I6" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="16" t="n">
+      <c r="C7" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="19" t="n">
+      <c r="E7" s="0" t="n">
         <v>1838</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="H7" s="16" t="s">
+      <c r="H7" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="I7" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="16" t="n">
+      <c r="C8" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="D8" s="13" t="n">
+      <c r="D8" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="E8" s="19" t="n">
+      <c r="E8" s="0" t="n">
         <v>1838</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="H8" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="I8" s="17" t="s">
+      <c r="I8" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="16" t="n">
+      <c r="C9" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="D9" s="13" t="n">
+      <c r="D9" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="E9" s="19" t="n">
+      <c r="E9" s="0" t="n">
         <v>1838</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="I9" s="17" t="s">
+      <c r="I9" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="16" t="n">
+      <c r="C10" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="D10" s="13" t="n">
+      <c r="D10" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="E10" s="19" t="n">
+      <c r="E10" s="0" t="n">
         <v>1838</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="H10" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="I10" s="17" t="s">
+      <c r="I10" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="18" t="n">
+      <c r="C11" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="D11" s="16" t="n">
+      <c r="D11" s="15" t="n">
         <v>5</v>
       </c>
-      <c r="E11" s="19" t="n">
+      <c r="E11" s="0" t="n">
         <v>1840</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="H11" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="I11" s="17" t="s">
+      <c r="I11" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="13" t="n">
+      <c r="C12" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="19" t="n">
+      <c r="E12" s="0" t="n">
         <v>1840</v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="G12" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="H12" s="16" t="s">
+      <c r="H12" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="I12" s="17" t="s">
+      <c r="I12" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="18" t="n">
+      <c r="C13" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="D13" s="16" t="n">
+      <c r="D13" s="15" t="n">
         <v>5</v>
       </c>
-      <c r="E13" s="19" t="n">
+      <c r="E13" s="0" t="n">
         <v>1840</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="G13" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="I13" s="17" t="s">
+      <c r="I13" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="16" t="n">
+      <c r="C14" s="15" t="n">
         <v>5</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="19" t="n">
+      <c r="E14" s="0" t="n">
         <v>1842</v>
       </c>
-      <c r="G14" s="17" t="s">
+      <c r="G14" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H14" s="16" t="s">
+      <c r="H14" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="I14" s="17" t="s">
+      <c r="I14" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="16" t="n">
+      <c r="C15" s="15" t="n">
         <v>5</v>
       </c>
-      <c r="D15" s="16" t="n">
+      <c r="D15" s="15" t="n">
         <v>7</v>
       </c>
-      <c r="E15" s="19" t="n">
+      <c r="E15" s="0" t="n">
         <v>1842</v>
       </c>
-      <c r="G15" s="17" t="s">
+      <c r="G15" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H15" s="16" t="s">
+      <c r="H15" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="I15" s="17" t="s">
+      <c r="I15" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="E16" s="19" t="n">
+      <c r="E16" s="0" t="n">
         <v>1829</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="G16" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="H16" s="16" t="s">
+      <c r="H16" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="I16" s="17" t="s">
+      <c r="I16" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="16" t="n">
+      <c r="C17" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="D17" s="18" t="n">
+      <c r="D17" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="E17" s="19" t="n">
+      <c r="E17" s="0" t="n">
         <v>1829</v>
       </c>
-      <c r="G17" s="17" t="s">
+      <c r="G17" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="H17" s="13" t="s">
+      <c r="H17" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="I17" s="17" t="s">
+      <c r="I17" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="E18" s="19" t="n">
+      <c r="E18" s="0" t="n">
         <v>1826</v>
       </c>
-      <c r="G18" s="17" t="s">
+      <c r="G18" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="H18" s="16" t="s">
+      <c r="H18" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="I18" s="17" t="s">
+      <c r="I18" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="16" t="n">
+      <c r="C19" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="D19" s="18" t="n">
+      <c r="D19" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="E19" s="19" t="n">
+      <c r="E19" s="0" t="n">
         <v>1826</v>
       </c>
-      <c r="G19" s="17" t="s">
+      <c r="G19" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="H19" s="16" t="s">
+      <c r="H19" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="I19" s="17" t="s">
+      <c r="I19" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="16" t="n">
+      <c r="C20" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="D20" s="18" t="n">
+      <c r="D20" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="E20" s="19" t="n">
+      <c r="E20" s="0" t="n">
         <v>1826</v>
       </c>
-      <c r="G20" s="17" t="s">
+      <c r="G20" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="H20" s="13" t="s">
+      <c r="H20" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="I20" s="17" t="s">
+      <c r="I20" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="16" t="n">
+      <c r="C21" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="D21" s="18" t="n">
+      <c r="D21" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="E21" s="19" t="n">
+      <c r="E21" s="0" t="n">
         <v>1826</v>
       </c>
-      <c r="G21" s="17" t="s">
+      <c r="G21" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="H21" s="13" t="s">
+      <c r="H21" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="I21" s="17" t="s">
+      <c r="I21" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="16" t="n">
+      <c r="C22" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="D22" s="18" t="n">
+      <c r="D22" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="E22" s="19" t="n">
+      <c r="E22" s="0" t="n">
         <v>1826</v>
       </c>
-      <c r="G22" s="17" t="s">
+      <c r="G22" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="H22" s="13" t="s">
+      <c r="H22" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="I22" s="17" t="s">
+      <c r="I22" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="16" t="n">
+      <c r="C23" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="D23" s="18" t="n">
+      <c r="D23" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="E23" s="19" t="n">
+      <c r="E23" s="0" t="n">
         <v>1826</v>
       </c>
-      <c r="G23" s="17" t="s">
+      <c r="G23" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="H23" s="13" t="s">
+      <c r="H23" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="I23" s="17" t="s">
+      <c r="I23" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="16" t="n">
+      <c r="C24" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="D24" s="18" t="n">
+      <c r="D24" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="E24" s="19" t="n">
+      <c r="E24" s="0" t="n">
         <v>1826</v>
       </c>
-      <c r="G24" s="17" t="s">
+      <c r="G24" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="H24" s="13" t="s">
+      <c r="H24" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="I24" s="17" t="s">
+      <c r="I24" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="16" t="n">
+      <c r="C25" s="15" t="n">
         <v>7</v>
       </c>
-      <c r="D25" s="16" t="s">
+      <c r="D25" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="E25" s="19" t="n">
+      <c r="E25" s="0" t="n">
         <v>1844</v>
       </c>
-      <c r="G25" s="17" t="s">
+      <c r="G25" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="H25" s="16" t="s">
+      <c r="H25" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="I25" s="17" t="s">
+      <c r="I25" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C26" s="16" t="n">
+      <c r="C26" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="D26" s="16" t="n">
+      <c r="D26" s="15" t="n">
         <v>2.4</v>
       </c>
-      <c r="E26" s="19" t="n">
+      <c r="E26" s="0" t="n">
         <v>1832</v>
       </c>
-      <c r="G26" s="17" t="s">
+      <c r="G26" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="H26" s="13" t="s">
+      <c r="H26" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="I26" s="17" t="s">
+      <c r="I26" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="16" t="n">
+      <c r="C27" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="D27" s="16" t="n">
+      <c r="D27" s="15" t="n">
         <v>2.4</v>
       </c>
-      <c r="E27" s="19" t="n">
+      <c r="E27" s="0" t="n">
         <v>1832</v>
       </c>
-      <c r="G27" s="17" t="s">
+      <c r="G27" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="H27" s="13" t="s">
+      <c r="H27" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="I27" s="17" t="s">
+      <c r="I27" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="16" t="n">
+      <c r="C28" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="D28" s="16" t="n">
+      <c r="D28" s="15" t="n">
         <v>2.4</v>
       </c>
-      <c r="E28" s="19" t="n">
+      <c r="E28" s="0" t="n">
         <v>1832</v>
       </c>
-      <c r="G28" s="17" t="s">
+      <c r="G28" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="H28" s="13" t="s">
+      <c r="H28" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="I28" s="17" t="s">
+      <c r="I28" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="17" t="s">
+      <c r="A29" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C29" s="16" t="n">
+      <c r="C29" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="D29" s="16" t="n">
+      <c r="D29" s="15" t="n">
         <v>2.4</v>
       </c>
-      <c r="E29" s="19" t="n">
+      <c r="E29" s="0" t="n">
         <v>1832</v>
       </c>
-      <c r="G29" s="17" t="s">
+      <c r="G29" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="H29" s="13" t="s">
+      <c r="H29" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="I29" s="17" t="s">
+      <c r="I29" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="17" t="s">
+      <c r="A30" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C30" s="16" t="n">
+      <c r="C30" s="15" t="n">
         <v>2.4</v>
       </c>
-      <c r="D30" s="16" t="n">
+      <c r="D30" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="E30" s="19" t="n">
+      <c r="E30" s="0" t="n">
         <v>1836</v>
       </c>
-      <c r="G30" s="17" t="s">
+      <c r="G30" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="H30" s="13" t="s">
+      <c r="H30" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="I30" s="17" t="s">
+      <c r="I30" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="17" t="s">
+      <c r="A31" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="16" t="n">
+      <c r="C31" s="15" t="n">
         <v>2.4</v>
       </c>
-      <c r="D31" s="16" t="n">
+      <c r="D31" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="E31" s="19" t="n">
+      <c r="E31" s="0" t="n">
         <v>1836</v>
       </c>
-      <c r="G31" s="17" t="s">
+      <c r="G31" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="H31" s="13" t="s">
+      <c r="H31" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="I31" s="17" t="s">
+      <c r="I31" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="17" t="s">
+      <c r="A32" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="16" t="n">
+      <c r="C32" s="15" t="n">
         <v>2.4</v>
       </c>
-      <c r="D32" s="16" t="n">
+      <c r="D32" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="E32" s="19" t="n">
+      <c r="E32" s="0" t="n">
         <v>1836</v>
       </c>
-      <c r="G32" s="17" t="s">
+      <c r="G32" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="H32" s="13" t="s">
+      <c r="H32" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="I32" s="17" t="s">
+      <c r="I32" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="17" t="s">
+      <c r="A33" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="C33" s="16" t="s">
+      <c r="C33" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="D33" s="16" t="s">
+      <c r="D33" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="E33" s="19" t="n">
+      <c r="E33" s="0" t="n">
         <v>1830</v>
       </c>
-      <c r="G33" s="17" t="s">
+      <c r="G33" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="H33" s="16" t="s">
+      <c r="H33" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="I33" s="17" t="s">
+      <c r="I33" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="17" t="s">
+      <c r="A34" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="C34" s="16" t="n">
+      <c r="C34" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="D34" s="18" t="n">
+      <c r="D34" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="E34" s="19" t="n">
+      <c r="E34" s="0" t="n">
         <v>1830</v>
       </c>
-      <c r="G34" s="17" t="s">
+      <c r="G34" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="H34" s="13" t="s">
+      <c r="H34" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="I34" s="17" t="s">
+      <c r="I34" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="17" t="s">
+      <c r="A35" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="C35" s="16" t="s">
+      <c r="C35" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="D35" s="16" t="s">
+      <c r="D35" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="E35" s="19" t="n">
+      <c r="E35" s="0" t="n">
         <v>1827</v>
       </c>
-      <c r="G35" s="17" t="s">
+      <c r="G35" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="H35" s="16" t="s">
+      <c r="H35" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="I35" s="17" t="s">
+      <c r="I35" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="17" t="s">
+      <c r="A36" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C36" s="16" t="n">
+      <c r="C36" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="D36" s="18" t="n">
+      <c r="D36" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="E36" s="19" t="n">
+      <c r="E36" s="0" t="n">
         <v>1827</v>
       </c>
-      <c r="G36" s="17" t="s">
+      <c r="G36" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="H36" s="16" t="s">
+      <c r="H36" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="I36" s="17" t="s">
+      <c r="I36" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="17" t="s">
+      <c r="A37" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="16" t="n">
+      <c r="C37" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="D37" s="18" t="n">
+      <c r="D37" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="E37" s="19" t="n">
+      <c r="E37" s="0" t="n">
         <v>1827</v>
       </c>
-      <c r="G37" s="17" t="s">
+      <c r="G37" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="H37" s="13" t="s">
+      <c r="H37" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="I37" s="17" t="s">
+      <c r="I37" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="17" t="s">
+      <c r="A38" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="16" t="n">
+      <c r="C38" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="D38" s="18" t="n">
+      <c r="D38" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="E38" s="19" t="n">
+      <c r="E38" s="0" t="n">
         <v>1827</v>
       </c>
-      <c r="G38" s="17" t="s">
+      <c r="G38" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="H38" s="13" t="s">
+      <c r="H38" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="I38" s="17" t="s">
+      <c r="I38" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="17" t="s">
+      <c r="A39" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C39" s="16" t="n">
+      <c r="C39" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="D39" s="18" t="n">
+      <c r="D39" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="E39" s="19" t="n">
+      <c r="E39" s="0" t="n">
         <v>1827</v>
       </c>
-      <c r="G39" s="17" t="s">
+      <c r="G39" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="H39" s="13" t="s">
+      <c r="H39" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="I39" s="17" t="s">
+      <c r="I39" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="17" t="s">
+      <c r="A40" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C40" s="16" t="n">
+      <c r="C40" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="D40" s="18" t="n">
+      <c r="D40" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="E40" s="19" t="n">
+      <c r="E40" s="0" t="n">
         <v>1827</v>
       </c>
-      <c r="G40" s="17" t="s">
+      <c r="G40" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="H40" s="13" t="s">
+      <c r="H40" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="I40" s="17" t="s">
+      <c r="I40" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="17" t="s">
+      <c r="A41" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B41" s="17" t="s">
+      <c r="B41" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C41" s="16" t="n">
+      <c r="C41" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="D41" s="18" t="n">
+      <c r="D41" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="E41" s="19" t="n">
+      <c r="E41" s="0" t="n">
         <v>1827</v>
       </c>
-      <c r="G41" s="17" t="s">
+      <c r="G41" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="H41" s="13" t="s">
+      <c r="H41" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="I41" s="17" t="s">
+      <c r="I41" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="17" t="s">
+      <c r="A42" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B42" s="17" t="s">
+      <c r="B42" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C42" s="16" t="n">
+      <c r="C42" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="D42" s="16" t="n">
+      <c r="D42" s="15" t="n">
         <v>2.4</v>
       </c>
-      <c r="E42" s="19" t="n">
-        <v>1833</v>
-      </c>
-      <c r="G42" s="17" t="s">
+      <c r="E42" s="0" t="n">
+        <v>2833</v>
+      </c>
+      <c r="G42" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="H42" s="13" t="s">
+      <c r="H42" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="I42" s="17" t="s">
+      <c r="I42" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="17" t="s">
+      <c r="A43" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B43" s="17" t="s">
+      <c r="B43" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C43" s="16" t="n">
+      <c r="C43" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="D43" s="16" t="n">
+      <c r="D43" s="15" t="n">
         <v>2.4</v>
       </c>
-      <c r="E43" s="19" t="n">
-        <v>1833</v>
-      </c>
-      <c r="G43" s="17" t="s">
+      <c r="E43" s="0" t="n">
+        <v>2833</v>
+      </c>
+      <c r="G43" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="H43" s="13" t="s">
+      <c r="H43" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="I43" s="17" t="s">
+      <c r="I43" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="17" t="s">
+      <c r="A44" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B44" s="17" t="s">
+      <c r="B44" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C44" s="16" t="n">
+      <c r="C44" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="D44" s="16" t="n">
+      <c r="D44" s="15" t="n">
         <v>2.4</v>
       </c>
-      <c r="E44" s="19" t="n">
-        <v>1833</v>
-      </c>
-      <c r="G44" s="17" t="s">
+      <c r="E44" s="0" t="n">
+        <v>2833</v>
+      </c>
+      <c r="G44" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="H44" s="13" t="s">
+      <c r="H44" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="I44" s="17" t="s">
+      <c r="I44" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="17" t="s">
+      <c r="A45" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B45" s="17" t="s">
+      <c r="B45" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C45" s="16" t="n">
+      <c r="C45" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="D45" s="16" t="n">
+      <c r="D45" s="15" t="n">
         <v>2.4</v>
       </c>
-      <c r="E45" s="19" t="n">
-        <v>1833</v>
-      </c>
-      <c r="G45" s="17" t="s">
+      <c r="E45" s="0" t="n">
+        <v>2833</v>
+      </c>
+      <c r="G45" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="H45" s="13" t="s">
+      <c r="H45" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="I45" s="17" t="s">
+      <c r="I45" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="17" t="s">
+      <c r="A46" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B46" s="17" t="s">
+      <c r="B46" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C46" s="16" t="n">
+      <c r="C46" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="D46" s="16" t="n">
+      <c r="D46" s="15" t="n">
         <v>2.4</v>
       </c>
-      <c r="E46" s="19" t="n">
-        <v>1833</v>
-      </c>
-      <c r="G46" s="17" t="s">
+      <c r="E46" s="0" t="n">
+        <v>3833</v>
+      </c>
+      <c r="G46" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="H46" s="13" t="s">
+      <c r="H46" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="I46" s="17" t="s">
+      <c r="I46" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="17" t="s">
+      <c r="A47" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B47" s="17" t="s">
+      <c r="B47" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C47" s="16" t="n">
+      <c r="C47" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="D47" s="16" t="n">
+      <c r="D47" s="15" t="n">
         <v>2.4</v>
       </c>
-      <c r="E47" s="19" t="n">
-        <v>1833</v>
-      </c>
-      <c r="G47" s="17" t="s">
+      <c r="E47" s="0" t="n">
+        <v>3833</v>
+      </c>
+      <c r="G47" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="H47" s="13" t="s">
+      <c r="H47" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="I47" s="17" t="s">
+      <c r="I47" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="17" t="s">
+      <c r="A48" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B48" s="17" t="s">
+      <c r="B48" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="16" t="n">
+      <c r="C48" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="D48" s="16" t="n">
+      <c r="D48" s="15" t="n">
         <v>2.4</v>
       </c>
-      <c r="E48" s="19" t="n">
-        <v>1833</v>
-      </c>
-      <c r="G48" s="17" t="s">
+      <c r="E48" s="0" t="n">
+        <v>3833</v>
+      </c>
+      <c r="G48" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="H48" s="13" t="s">
+      <c r="H48" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="I48" s="17" t="s">
+      <c r="I48" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="17" t="s">
+      <c r="A49" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B49" s="17" t="s">
+      <c r="B49" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C49" s="16" t="n">
+      <c r="C49" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="D49" s="16" t="n">
+      <c r="D49" s="15" t="n">
         <v>2.4</v>
       </c>
-      <c r="E49" s="19" t="n">
-        <v>1833</v>
-      </c>
-      <c r="G49" s="17" t="s">
+      <c r="E49" s="0" t="n">
+        <v>3833</v>
+      </c>
+      <c r="G49" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="H49" s="13" t="s">
+      <c r="H49" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="I49" s="17" t="s">
+      <c r="I49" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="17" t="s">
+      <c r="A50" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B50" s="17" t="s">
+      <c r="B50" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="C50" s="18" t="n">
+      <c r="C50" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="D50" s="16" t="s">
+      <c r="D50" s="15" t="s">
         <v>55</v>
       </c>
       <c r="E50" s="0" t="n">
-        <v>1835</v>
-      </c>
-      <c r="G50" s="17" t="s">
+        <v>3835</v>
+      </c>
+      <c r="G50" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="H50" s="16" t="s">
+      <c r="H50" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="I50" s="17" t="s">
+      <c r="I50" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="17" t="s">
+      <c r="A51" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B51" s="17" t="s">
+      <c r="B51" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="C51" s="18" t="n">
+      <c r="C51" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="D51" s="16" t="s">
+      <c r="D51" s="15" t="s">
         <v>55</v>
       </c>
       <c r="E51" s="0" t="n">
-        <v>1835</v>
-      </c>
-      <c r="G51" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="H51" s="16" t="s">
+        <v>2835</v>
+      </c>
+      <c r="G51" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="H51" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="I51" s="17" t="s">
+      <c r="I51" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="17" t="s">
+      <c r="A52" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B52" s="17" t="s">
+      <c r="B52" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C52" s="18" t="n">
+      <c r="C52" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="D52" s="16" t="s">
+      <c r="D52" s="15" t="s">
         <v>55</v>
       </c>
       <c r="E52" s="0" t="n">
-        <v>1833</v>
-      </c>
-      <c r="G52" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="H52" s="16" t="s">
+        <v>3833</v>
+      </c>
+      <c r="G52" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="H52" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="I52" s="17" t="s">
+      <c r="I52" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="17" t="s">
+      <c r="A53" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B53" s="17" t="s">
+      <c r="B53" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C53" s="18" t="n">
+      <c r="C53" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="D53" s="16" t="s">
+      <c r="D53" s="15" t="s">
         <v>55</v>
       </c>
       <c r="E53" s="0" t="n">
-        <v>1833</v>
-      </c>
-      <c r="G53" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="H53" s="16" t="s">
+        <v>2833</v>
+      </c>
+      <c r="G53" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="H53" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="I53" s="17" t="s">
+      <c r="I53" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="17" t="s">
+      <c r="A54" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B54" s="17" t="s">
+      <c r="B54" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C54" s="16" t="n">
+      <c r="C54" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="D54" s="16" t="n">
+      <c r="D54" s="15" t="n">
         <v>2.4</v>
       </c>
       <c r="E54" s="0" t="n">
-        <v>1833</v>
-      </c>
-      <c r="G54" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="H54" s="16" t="s">
+        <v>3833</v>
+      </c>
+      <c r="G54" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="H54" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="I54" s="17" t="s">
+      <c r="I54" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="17" t="s">
+      <c r="A55" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B55" s="17" t="s">
+      <c r="B55" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C55" s="16" t="n">
+      <c r="C55" s="15" t="n">
         <v>1.6</v>
       </c>
-      <c r="D55" s="16" t="n">
+      <c r="D55" s="15" t="n">
         <v>2.4</v>
       </c>
       <c r="E55" s="0" t="n">
-        <v>1833</v>
-      </c>
-      <c r="G55" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="H55" s="16" t="s">
+        <v>2833</v>
+      </c>
+      <c r="G55" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="H55" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="I55" s="17" t="s">
+      <c r="I55" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="17" t="s">
+      <c r="A56" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B56" s="17" t="s">
+      <c r="B56" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C56" s="16" t="n">
+      <c r="C56" s="15" t="n">
         <v>2.4</v>
       </c>
-      <c r="D56" s="16" t="n">
+      <c r="D56" s="15" t="n">
         <v>3</v>
       </c>
       <c r="E56" s="0" t="n">
-        <v>1837</v>
-      </c>
-      <c r="G56" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="H56" s="13" t="s">
+        <v>3837</v>
+      </c>
+      <c r="G56" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="H56" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="I56" s="17" t="s">
+      <c r="I56" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="17" t="s">
+      <c r="A57" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B57" s="17" t="s">
+      <c r="B57" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C57" s="16" t="n">
+      <c r="C57" s="15" t="n">
         <v>2.4</v>
       </c>
-      <c r="D57" s="16" t="n">
+      <c r="D57" s="15" t="n">
         <v>3</v>
       </c>
       <c r="E57" s="0" t="n">
-        <v>1837</v>
-      </c>
-      <c r="G57" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="H57" s="13" t="s">
+        <v>2837</v>
+      </c>
+      <c r="G57" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="H57" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="I57" s="17" t="s">
+      <c r="I57" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="17" t="s">
+      <c r="A58" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B58" s="17" t="s">
+      <c r="B58" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C58" s="16" t="n">
+      <c r="C58" s="15" t="n">
         <v>2.4</v>
       </c>
-      <c r="D58" s="16" t="n">
+      <c r="D58" s="15" t="n">
         <v>3</v>
       </c>
       <c r="E58" s="0" t="n">
-        <v>1837</v>
-      </c>
-      <c r="G58" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="H58" s="13" t="s">
+        <v>3837</v>
+      </c>
+      <c r="G58" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="H58" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="I58" s="17" t="s">
+      <c r="I58" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="17" t="s">
+      <c r="A59" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B59" s="17" t="s">
+      <c r="B59" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C59" s="16" t="n">
+      <c r="C59" s="15" t="n">
         <v>2.4</v>
       </c>
-      <c r="D59" s="16" t="n">
+      <c r="D59" s="15" t="n">
         <v>3</v>
       </c>
       <c r="E59" s="0" t="n">
-        <v>1837</v>
-      </c>
-      <c r="G59" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="H59" s="13" t="s">
+        <v>2837</v>
+      </c>
+      <c r="G59" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="H59" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="I59" s="17" t="s">
+      <c r="I59" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="17" t="s">
+      <c r="A60" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B60" s="17" t="s">
+      <c r="B60" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C60" s="16" t="n">
+      <c r="C60" s="15" t="n">
         <v>2.4</v>
       </c>
-      <c r="D60" s="16" t="n">
+      <c r="D60" s="15" t="n">
         <v>3</v>
       </c>
       <c r="E60" s="0" t="n">
-        <v>1837</v>
-      </c>
-      <c r="G60" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="H60" s="13" t="s">
+        <v>3837</v>
+      </c>
+      <c r="G60" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="H60" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="I60" s="17" t="s">
+      <c r="I60" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="17" t="s">
+      <c r="A61" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B61" s="17" t="s">
+      <c r="B61" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C61" s="16" t="n">
+      <c r="C61" s="15" t="n">
         <v>2.4</v>
       </c>
-      <c r="D61" s="16" t="n">
+      <c r="D61" s="15" t="n">
         <v>3</v>
       </c>
       <c r="E61" s="0" t="n">
-        <v>1837</v>
-      </c>
-      <c r="G61" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="H61" s="13" t="s">
+        <v>2837</v>
+      </c>
+      <c r="G61" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="H61" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="I61" s="17" t="s">
+      <c r="I61" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="17" t="s">
+      <c r="A62" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B62" s="17" t="s">
+      <c r="B62" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C62" s="16" t="n">
+      <c r="C62" s="15" t="n">
         <v>2.4</v>
       </c>
-      <c r="D62" s="16" t="s">
+      <c r="D62" s="15" t="s">
         <v>55</v>
       </c>
       <c r="E62" s="0" t="n">
-        <v>1837</v>
-      </c>
-      <c r="G62" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="H62" s="16" t="s">
+        <v>3837</v>
+      </c>
+      <c r="G62" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="H62" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="I62" s="17" t="s">
+      <c r="I62" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="17" t="s">
+      <c r="A63" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B63" s="17" t="s">
+      <c r="B63" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C63" s="16" t="n">
+      <c r="C63" s="15" t="n">
         <v>2.4</v>
       </c>
-      <c r="D63" s="16" t="s">
+      <c r="D63" s="15" t="s">
         <v>55</v>
       </c>
       <c r="E63" s="0" t="n">
-        <v>1837</v>
-      </c>
-      <c r="G63" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="H63" s="16" t="s">
+        <v>2837</v>
+      </c>
+      <c r="G63" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="H63" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="I63" s="17" t="s">
+      <c r="I63" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="17" t="s">
+      <c r="A64" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B64" s="17" t="s">
+      <c r="B64" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C64" s="16" t="n">
+      <c r="C64" s="15" t="n">
         <v>2.4</v>
       </c>
-      <c r="D64" s="16" t="n">
+      <c r="D64" s="15" t="n">
         <v>3</v>
       </c>
       <c r="E64" s="0" t="n">
-        <v>1837</v>
-      </c>
-      <c r="G64" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="H64" s="16" t="s">
+        <v>3837</v>
+      </c>
+      <c r="G64" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="H64" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="I64" s="17" t="s">
+      <c r="I64" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="17" t="s">
+      <c r="A65" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B65" s="17" t="s">
+      <c r="B65" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C65" s="16" t="n">
+      <c r="C65" s="15" t="n">
         <v>2.4</v>
       </c>
-      <c r="D65" s="16" t="n">
+      <c r="D65" s="15" t="n">
         <v>3</v>
       </c>
       <c r="E65" s="0" t="n">
-        <v>1837</v>
-      </c>
-      <c r="G65" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="H65" s="16" t="s">
+        <v>2837</v>
+      </c>
+      <c r="G65" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="H65" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="I65" s="17" t="s">
+      <c r="I65" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="17" t="s">
+      <c r="A66" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B66" s="17" t="s">
+      <c r="B66" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C66" s="13" t="n">
+      <c r="C66" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="D66" s="16" t="s">
+      <c r="D66" s="15" t="s">
         <v>55</v>
       </c>
       <c r="E66" s="0" t="n">
-        <v>1839</v>
-      </c>
-      <c r="G66" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="H66" s="16" t="s">
+        <v>3839</v>
+      </c>
+      <c r="G66" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="H66" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="I66" s="17" t="s">
+      <c r="I66" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="17" t="s">
+      <c r="A67" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B67" s="17" t="s">
+      <c r="B67" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C67" s="13" t="n">
+      <c r="C67" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="D67" s="16" t="s">
+      <c r="D67" s="15" t="s">
         <v>55</v>
       </c>
       <c r="E67" s="0" t="n">
-        <v>1839</v>
-      </c>
-      <c r="G67" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="H67" s="16" t="s">
+        <v>2839</v>
+      </c>
+      <c r="G67" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="H67" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="I67" s="17" t="s">
+      <c r="I67" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="17" t="s">
+      <c r="A68" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B68" s="17" t="s">
+      <c r="B68" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C68" s="13" t="n">
+      <c r="C68" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="D68" s="13" t="n">
+      <c r="D68" s="15" t="n">
         <v>4</v>
       </c>
       <c r="E68" s="0" t="n">
-        <v>1839</v>
-      </c>
-      <c r="G68" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="H68" s="16" t="s">
+        <v>3839</v>
+      </c>
+      <c r="G68" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="H68" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="I68" s="17" t="s">
+      <c r="I68" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="17" t="s">
+      <c r="A69" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B69" s="17" t="s">
+      <c r="B69" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C69" s="13" t="n">
+      <c r="C69" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="D69" s="13" t="n">
+      <c r="D69" s="15" t="n">
         <v>4</v>
       </c>
       <c r="E69" s="0" t="n">
-        <v>1839</v>
-      </c>
-      <c r="G69" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="H69" s="16" t="s">
+        <v>2839</v>
+      </c>
+      <c r="G69" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="H69" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="I69" s="17" t="s">
+      <c r="I69" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="17" t="s">
+      <c r="A70" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B70" s="17" t="s">
+      <c r="B70" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C70" s="13" t="n">
+      <c r="C70" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="D70" s="13" t="n">
+      <c r="D70" s="15" t="n">
         <v>4</v>
       </c>
       <c r="E70" s="0" t="n">
-        <v>1839</v>
-      </c>
-      <c r="G70" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="H70" s="13" t="s">
+        <v>3839</v>
+      </c>
+      <c r="G70" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="H70" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="I70" s="17" t="s">
+      <c r="I70" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="17" t="s">
+      <c r="A71" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B71" s="17" t="s">
+      <c r="B71" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C71" s="13" t="n">
+      <c r="C71" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="D71" s="13" t="n">
+      <c r="D71" s="15" t="n">
         <v>4</v>
       </c>
       <c r="E71" s="0" t="n">
-        <v>1839</v>
-      </c>
-      <c r="G71" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="H71" s="13" t="s">
+        <v>2839</v>
+      </c>
+      <c r="G71" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="H71" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="I71" s="17" t="s">
+      <c r="I71" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="17" t="s">
+      <c r="A72" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B72" s="17" t="s">
+      <c r="B72" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C72" s="13" t="n">
+      <c r="C72" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="D72" s="13" t="n">
+      <c r="D72" s="15" t="n">
         <v>4</v>
       </c>
       <c r="E72" s="0" t="n">
-        <v>1839</v>
-      </c>
-      <c r="G72" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="H72" s="13" t="s">
+        <v>3839</v>
+      </c>
+      <c r="G72" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="H72" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="I72" s="17" t="s">
+      <c r="I72" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="17" t="s">
+      <c r="A73" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B73" s="17" t="s">
+      <c r="B73" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C73" s="13" t="n">
+      <c r="C73" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="D73" s="13" t="n">
+      <c r="D73" s="15" t="n">
         <v>4</v>
       </c>
       <c r="E73" s="0" t="n">
-        <v>1839</v>
-      </c>
-      <c r="G73" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="H73" s="13" t="s">
+        <v>2839</v>
+      </c>
+      <c r="G73" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="H73" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="I73" s="17" t="s">
+      <c r="I73" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="17" t="s">
+      <c r="A74" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B74" s="17" t="s">
+      <c r="B74" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C74" s="18" t="n">
+      <c r="C74" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="D74" s="16" t="n">
+      <c r="D74" s="15" t="n">
         <v>5</v>
       </c>
       <c r="E74" s="0" t="n">
-        <v>1841</v>
-      </c>
-      <c r="G74" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="H74" s="16" t="s">
+        <v>3841</v>
+      </c>
+      <c r="G74" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="H74" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="I74" s="17" t="s">
+      <c r="I74" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="17" t="s">
+      <c r="A75" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B75" s="17" t="s">
+      <c r="B75" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C75" s="18" t="n">
+      <c r="C75" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="D75" s="16" t="n">
+      <c r="D75" s="15" t="n">
         <v>5</v>
       </c>
       <c r="E75" s="0" t="n">
-        <v>1841</v>
-      </c>
-      <c r="G75" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="H75" s="16" t="s">
+        <v>2841</v>
+      </c>
+      <c r="G75" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="H75" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="I75" s="17" t="s">
+      <c r="I75" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="17" t="s">
+      <c r="A76" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B76" s="17" t="s">
+      <c r="B76" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C76" s="13" t="n">
+      <c r="C76" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="D76" s="16" t="s">
+      <c r="D76" s="15" t="s">
         <v>55</v>
       </c>
       <c r="E76" s="0" t="n">
-        <v>1841</v>
-      </c>
-      <c r="G76" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="H76" s="16" t="s">
+        <v>3841</v>
+      </c>
+      <c r="G76" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="H76" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="I76" s="17" t="s">
+      <c r="I76" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="17" t="s">
+      <c r="A77" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B77" s="17" t="s">
+      <c r="B77" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C77" s="13" t="n">
+      <c r="C77" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="D77" s="16" t="s">
+      <c r="D77" s="15" t="s">
         <v>55</v>
       </c>
       <c r="E77" s="0" t="n">
-        <v>1841</v>
-      </c>
-      <c r="G77" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="H77" s="16" t="s">
+        <v>2841</v>
+      </c>
+      <c r="G77" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="H77" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="I77" s="17" t="s">
+      <c r="I77" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="17" t="s">
+      <c r="A78" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B78" s="17" t="s">
+      <c r="B78" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C78" s="18" t="n">
+      <c r="C78" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="D78" s="16" t="n">
+      <c r="D78" s="15" t="n">
         <v>5</v>
       </c>
       <c r="E78" s="0" t="n">
-        <v>1841</v>
-      </c>
-      <c r="G78" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="H78" s="16" t="s">
+        <v>3841</v>
+      </c>
+      <c r="G78" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="H78" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="I78" s="17" t="s">
+      <c r="I78" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="17" t="s">
+      <c r="A79" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B79" s="17" t="s">
+      <c r="B79" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C79" s="18" t="n">
+      <c r="C79" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="D79" s="16" t="n">
+      <c r="D79" s="15" t="n">
         <v>5</v>
       </c>
       <c r="E79" s="0" t="n">
-        <v>1841</v>
-      </c>
-      <c r="G79" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="H79" s="16" t="s">
+        <v>2841</v>
+      </c>
+      <c r="G79" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="H79" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="I79" s="17" t="s">
+      <c r="I79" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="17" t="s">
+      <c r="A80" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B80" s="17" t="s">
+      <c r="B80" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C80" s="13" t="n">
+      <c r="C80" s="15" t="n">
         <v>5</v>
       </c>
-      <c r="D80" s="16" t="s">
+      <c r="D80" s="15" t="s">
         <v>55</v>
       </c>
       <c r="E80" s="0" t="n">
-        <v>1843</v>
-      </c>
-      <c r="G80" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="H80" s="16" t="s">
+        <v>3843</v>
+      </c>
+      <c r="G80" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="H80" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="I80" s="17" t="s">
+      <c r="I80" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="17" t="s">
+      <c r="A81" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B81" s="17" t="s">
+      <c r="B81" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C81" s="13" t="n">
+      <c r="C81" s="15" t="n">
         <v>5</v>
       </c>
-      <c r="D81" s="16" t="s">
+      <c r="D81" s="15" t="s">
         <v>55</v>
       </c>
       <c r="E81" s="0" t="n">
-        <v>1843</v>
-      </c>
-      <c r="G81" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="H81" s="16" t="s">
+        <v>2843</v>
+      </c>
+      <c r="G81" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="H81" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="I81" s="17" t="s">
+      <c r="I81" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="17" t="s">
+      <c r="A82" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B82" s="17" t="s">
+      <c r="B82" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C82" s="13" t="n">
+      <c r="C82" s="15" t="n">
         <v>5</v>
       </c>
-      <c r="D82" s="13" t="n">
+      <c r="D82" s="15" t="n">
         <v>7</v>
       </c>
       <c r="E82" s="0" t="n">
-        <v>1843</v>
-      </c>
-      <c r="G82" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="H82" s="16" t="s">
+        <v>3843</v>
+      </c>
+      <c r="G82" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="H82" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="I82" s="17" t="s">
+      <c r="I82" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="17" t="s">
+      <c r="A83" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B83" s="17" t="s">
+      <c r="B83" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C83" s="13" t="n">
+      <c r="C83" s="15" t="n">
         <v>5</v>
       </c>
-      <c r="D83" s="13" t="n">
+      <c r="D83" s="15" t="n">
         <v>7</v>
       </c>
       <c r="E83" s="0" t="n">
-        <v>1843</v>
-      </c>
-      <c r="G83" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="H83" s="16" t="s">
+        <v>2843</v>
+      </c>
+      <c r="G83" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="H83" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="I83" s="17" t="s">
+      <c r="I83" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="17" t="s">
+      <c r="A84" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B84" s="17" t="s">
+      <c r="B84" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C84" s="13" t="n">
+      <c r="C84" s="15" t="n">
         <v>7</v>
       </c>
-      <c r="D84" s="16" t="s">
+      <c r="D84" s="15" t="s">
         <v>55</v>
       </c>
       <c r="E84" s="0" t="n">
-        <v>1845</v>
-      </c>
-      <c r="G84" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="H84" s="16" t="s">
+        <v>3845</v>
+      </c>
+      <c r="G84" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="H84" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="I84" s="17" t="s">
+      <c r="I84" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="17" t="s">
+      <c r="A85" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B85" s="17" t="s">
+      <c r="B85" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C85" s="13" t="n">
+      <c r="C85" s="15" t="n">
         <v>7</v>
       </c>
-      <c r="D85" s="16" t="s">
+      <c r="D85" s="15" t="s">
         <v>55</v>
       </c>
       <c r="E85" s="0" t="n">
-        <v>1845</v>
-      </c>
-      <c r="G85" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="H85" s="16" t="s">
+        <v>2845</v>
+      </c>
+      <c r="G85" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="H85" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="I85" s="17" t="s">
+      <c r="I85" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="17" t="s">
+      <c r="A86" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B86" s="17" t="s">
+      <c r="B86" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="C86" s="16" t="s">
+      <c r="C86" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="D86" s="16" t="s">
+      <c r="D86" s="15" t="s">
         <v>55</v>
       </c>
       <c r="E86" s="0" t="n">
         <v>1831</v>
       </c>
-      <c r="G86" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="H86" s="16" t="s">
+      <c r="G86" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="H86" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="I86" s="17" t="s">
+      <c r="I86" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="17" t="s">
+      <c r="A87" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B87" s="17" t="s">
+      <c r="B87" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="C87" s="16" t="n">
+      <c r="C87" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="D87" s="18" t="n">
+      <c r="D87" s="15" t="n">
         <v>1.6</v>
       </c>
       <c r="E87" s="0" t="n">
         <v>1831</v>
       </c>
-      <c r="G87" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="H87" s="13" t="s">
+      <c r="G87" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="H87" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="I87" s="17" t="s">
+      <c r="I87" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="17" t="s">
+      <c r="A88" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B88" s="17" t="s">
+      <c r="B88" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="C88" s="16" t="s">
+      <c r="C88" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="D88" s="16" t="s">
+      <c r="D88" s="15" t="s">
         <v>55</v>
       </c>
       <c r="E88" s="0" t="n">
         <v>1828</v>
       </c>
-      <c r="G88" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="H88" s="16" t="s">
+      <c r="G88" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H88" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="I88" s="17" t="s">
+      <c r="I88" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="17" t="s">
+      <c r="A89" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B89" s="17" t="s">
+      <c r="B89" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C89" s="16" t="n">
+      <c r="C89" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="D89" s="18" t="n">
+      <c r="D89" s="15" t="n">
         <v>1.6</v>
       </c>
       <c r="E89" s="0" t="n">
         <v>1828</v>
       </c>
-      <c r="G89" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="H89" s="16" t="s">
+      <c r="G89" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H89" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="I89" s="17" t="s">
+      <c r="I89" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="17" t="s">
+      <c r="A90" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B90" s="17" t="s">
+      <c r="B90" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C90" s="16" t="n">
+      <c r="C90" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="D90" s="18" t="n">
+      <c r="D90" s="15" t="n">
         <v>1.6</v>
       </c>
       <c r="E90" s="0" t="n">
         <v>1828</v>
       </c>
-      <c r="G90" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="H90" s="13" t="s">
+      <c r="G90" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H90" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="I90" s="17" t="s">
+      <c r="I90" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="17" t="s">
+      <c r="A91" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B91" s="17" t="s">
+      <c r="B91" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C91" s="16" t="n">
+      <c r="C91" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="D91" s="18" t="n">
+      <c r="D91" s="15" t="n">
         <v>1.6</v>
       </c>
       <c r="E91" s="0" t="n">
         <v>1828</v>
       </c>
-      <c r="G91" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="H91" s="13" t="s">
+      <c r="G91" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H91" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="I91" s="17" t="s">
+      <c r="I91" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="17" t="s">
+      <c r="A92" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B92" s="17" t="s">
+      <c r="B92" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C92" s="16" t="n">
+      <c r="C92" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="D92" s="18" t="n">
+      <c r="D92" s="15" t="n">
         <v>1.6</v>
       </c>
       <c r="E92" s="0" t="n">
         <v>1828</v>
       </c>
-      <c r="G92" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="H92" s="13" t="s">
+      <c r="G92" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H92" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="I92" s="17" t="s">
+      <c r="I92" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="17" t="s">
+      <c r="A93" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B93" s="17" t="s">
+      <c r="B93" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C93" s="16" t="n">
+      <c r="C93" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="D93" s="18" t="n">
+      <c r="D93" s="15" t="n">
         <v>1.6</v>
       </c>
       <c r="E93" s="0" t="n">
         <v>1828</v>
       </c>
-      <c r="G93" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="H93" s="13" t="s">
+      <c r="G93" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H93" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="I93" s="17" t="s">
+      <c r="I93" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="17" t="s">
+      <c r="A94" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B94" s="17" t="s">
+      <c r="B94" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C94" s="16" t="n">
+      <c r="C94" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="D94" s="18" t="n">
+      <c r="D94" s="15" t="n">
         <v>1.6</v>
       </c>
       <c r="E94" s="0" t="n">
         <v>1828</v>
       </c>
-      <c r="G94" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="H94" s="13" t="s">
+      <c r="G94" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H94" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="I94" s="17" t="s">
+      <c r="I94" s="0" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3849,10 +3937,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="61.5789473684211"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.9433198380567"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.6032388663968"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.1295546558704"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.3441295546559"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.9554655870445"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3923,10 +4011,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="61.5789473684211"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.9433198380567"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.6153846153846"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.1295546558704"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.3441295546559"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="84.4089068825911"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3997,10 +4085,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="61.5789473684211"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.9433198380567"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.1295546558704"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.3441295546559"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="77.0202429149798"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4071,8 +4159,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="38.9352226720648"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="172.004048582996"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="39.2064777327935"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="173.534412955466"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="5" width="9.4251012145749"/>
   </cols>
   <sheetData>
@@ -4132,8 +4220,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="50.0688259109312"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="33.5425101214575"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="50.5587044534413"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="33.8502024291498"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="5" width="9.4251012145749"/>
   </cols>
   <sheetData>
@@ -4193,10 +4281,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.4372469635628"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.8016194331984"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.2105263157895"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.9878542510121"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.3076923076923"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.5991902834008"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4261,14 +4349,14 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="39.5425101214575"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="154.372469635628"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="39.8502024291498"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="155.748987854251"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="5" width="9.4251012145749"/>
   </cols>
   <sheetData>
@@ -4280,7 +4368,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -4288,7 +4376,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="66.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -4296,7 +4384,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -4323,13 +4411,13 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="51.0445344129555"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="78.7165991902834"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="51.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="79.3765182186235"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="5" width="9.4251012145749"/>
   </cols>
   <sheetData>
@@ -4342,30 +4430,30 @@
       </c>
       <c r="C1" s="0"/>
     </row>
-    <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" s="0"/>
     </row>
-    <row r="3" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="66.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="0"/>
     </row>
-    <row r="4" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="0"/>
     </row>

</xml_diff>

<commit_message>
PROS-5308 - BATRU - P3 placement bug - Empty Competitor
</commit_message>
<xml_diff>
--- a/Projects/MARSRU_PROD/Data/MARS must-range targets.xlsx
+++ b/Projects/MARSRU_PROD/Data/MARS must-range targets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="1648" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="111">
   <si>
     <t xml:space="preserve">Store type</t>
   </si>
@@ -482,9 +482,7 @@
 Grocery Магазин у дома (450-599),
 Grocery Магазин у дома (600-999)
 Grocery Дискаунтер (&lt;300),
-Grocery Дискаунтер (300-999),
-Grocery BIG BOXES (1000-2499),
-Grocery BIG BOXES (2500+)</t>
+Grocery Дискаунтер (300-999)</t>
   </si>
   <si>
     <t xml:space="preserve">4607065377984,
@@ -495,6 +493,17 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">Grocery Магазин у дома (&lt;100),
+Grocery Магазин у дома (100-299),
+Grocery Магазин у дома (300-449),
+Grocery Магазин у дома (450-599),
+Grocery Магазин у дома (600-999)
+Grocery Дискаунтер (&lt;300),
+Grocery Дискаунтер (300-999),
+Grocery BIG BOXES (1000-2499),
+Grocery BIG BOXES (2500+)</t>
+  </si>
+  <si>
     <t xml:space="preserve">4607065376048,
 4607065002862,
 4607065377984,
@@ -503,12 +512,84 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">4607065376048,
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">4607065376048,
 4607065002862,
-4607065002862,
-4607065375119,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">4607065371227,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">4607065375119,
 4607065004071
 </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Grocery BIG BOXES (1000-2499),
+Grocery BIG BOXES (2500+)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">4607065377984
+4607065001612
+5998749106877
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">5998749123072
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">5000159438735</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">4607065003999,
@@ -793,7 +874,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -819,15 +900,25 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val=""/>
-      <family val="1"/>
-      <charset val="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val=""/>
-      <family val="1"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="4">
@@ -934,10 +1025,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1034,7 +1125,7 @@
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF00B050"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -1059,9 +1150,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.8137651821862"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="59.7732793522267"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.1336032388664"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.3076923076923"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.0931174089069"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1171,60 +1262,60 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.4534412955466"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.4493927125506"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="82.9109311740891"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.8825910931174"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.9878542510121"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.6599190283401"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.4251012145749"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
+    <row r="1" customFormat="false" ht="94.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="121.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>31</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>6</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="121.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>6</v>
+        <v>31</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="121.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="66.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1246,14 +1337,14 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.2024291497976"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.0607287449393"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="118.793522267206"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.6315789473684"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.5951417004049"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="119.866396761134"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.4251012145749"/>
   </cols>
   <sheetData>
@@ -1270,35 +1361,35 @@
     </row>
     <row r="2" customFormat="false" ht="356.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="350.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="350.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1347,8 +1438,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.9554655870445"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.2753036437247"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.7449392712551"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1357,79 +1448,79 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="14" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>43</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="14" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="14" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1450,109 +1541,109 @@
   </sheetPr>
   <dimension ref="A1:I94"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.6396761133603"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.2793522267206"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="15" width="28.8137651821862"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="15" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8542510121457"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.5991902834008"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="15" width="29.0283400809717"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="15" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.3522267206478"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.53441295546559"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="42.5263157894737"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="42.9554655870445"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.8137651821862"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.4251012145749"/>
   </cols>
   <sheetData>
     <row r="1" s="15" customFormat="true" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F1" s="17"/>
       <c r="G1" s="18" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="I1" s="19" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="20" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C2" s="15" t="n">
         <v>1.6</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>1834</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C3" s="15" t="n">
         <v>1.6</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>1832</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C4" s="15" t="n">
         <v>1.6</v>
@@ -1564,47 +1655,47 @@
         <v>1832</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C5" s="15" t="n">
         <v>2.4</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>1836</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C6" s="15" t="n">
         <v>2.4</v>
@@ -1616,47 +1707,47 @@
         <v>1836</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C7" s="15" t="n">
         <v>3</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>1838</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C8" s="15" t="n">
         <v>3</v>
@@ -1668,21 +1759,21 @@
         <v>1838</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C9" s="15" t="n">
         <v>3</v>
@@ -1694,21 +1785,21 @@
         <v>1838</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C10" s="15" t="n">
         <v>3</v>
@@ -1720,21 +1811,21 @@
         <v>1838</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C11" s="15" t="n">
         <v>4</v>
@@ -1746,47 +1837,47 @@
         <v>1840</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C12" s="15" t="n">
         <v>4</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>1840</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C13" s="15" t="n">
         <v>4</v>
@@ -1798,47 +1889,47 @@
         <v>1840</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C14" s="15" t="n">
         <v>5</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>1842</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C15" s="15" t="n">
         <v>5</v>
@@ -1850,47 +1941,47 @@
         <v>1842</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>1829</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C17" s="15" t="n">
         <v>0</v>
@@ -1902,47 +1993,47 @@
         <v>1829</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>1826</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C19" s="15" t="n">
         <v>0</v>
@@ -1954,21 +2045,21 @@
         <v>1826</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C20" s="15" t="n">
         <v>0</v>
@@ -1980,21 +2071,21 @@
         <v>1826</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C21" s="15" t="n">
         <v>0</v>
@@ -2006,21 +2097,21 @@
         <v>1826</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C22" s="15" t="n">
         <v>0</v>
@@ -2032,21 +2123,21 @@
         <v>1826</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C23" s="15" t="n">
         <v>0</v>
@@ -2058,21 +2149,21 @@
         <v>1826</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C24" s="15" t="n">
         <v>0</v>
@@ -2084,47 +2175,47 @@
         <v>1826</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C25" s="15" t="n">
         <v>7</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>1844</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C26" s="15" t="n">
         <v>1.6</v>
@@ -2136,21 +2227,21 @@
         <v>1832</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C27" s="15" t="n">
         <v>1.6</v>
@@ -2162,21 +2253,21 @@
         <v>1832</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C28" s="15" t="n">
         <v>1.6</v>
@@ -2188,21 +2279,21 @@
         <v>1832</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C29" s="15" t="n">
         <v>1.6</v>
@@ -2214,21 +2305,21 @@
         <v>1832</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C30" s="15" t="n">
         <v>2.4</v>
@@ -2240,21 +2331,21 @@
         <v>1836</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C31" s="15" t="n">
         <v>2.4</v>
@@ -2266,21 +2357,21 @@
         <v>1836</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C32" s="15" t="n">
         <v>2.4</v>
@@ -2292,47 +2383,47 @@
         <v>1836</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E33" s="0" t="n">
         <v>1830</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C34" s="15" t="n">
         <v>0</v>
@@ -2344,47 +2435,47 @@
         <v>1830</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E35" s="0" t="n">
         <v>1827</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C36" s="15" t="n">
         <v>0</v>
@@ -2396,21 +2487,21 @@
         <v>1827</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C37" s="15" t="n">
         <v>0</v>
@@ -2422,21 +2513,21 @@
         <v>1827</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C38" s="15" t="n">
         <v>0</v>
@@ -2448,21 +2539,21 @@
         <v>1827</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I38" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C39" s="15" t="n">
         <v>0</v>
@@ -2474,21 +2565,21 @@
         <v>1827</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I39" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C40" s="15" t="n">
         <v>0</v>
@@ -2500,21 +2591,21 @@
         <v>1827</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I40" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C41" s="15" t="n">
         <v>0</v>
@@ -2526,21 +2617,21 @@
         <v>1827</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I41" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C42" s="15" t="n">
         <v>1.6</v>
@@ -2552,21 +2643,21 @@
         <v>2833</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I42" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C43" s="15" t="n">
         <v>1.6</v>
@@ -2578,21 +2669,21 @@
         <v>2833</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I43" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C44" s="15" t="n">
         <v>1.6</v>
@@ -2604,21 +2695,21 @@
         <v>2833</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I44" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C45" s="15" t="n">
         <v>1.6</v>
@@ -2630,21 +2721,21 @@
         <v>2833</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I45" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C46" s="15" t="n">
         <v>1.6</v>
@@ -2656,21 +2747,21 @@
         <v>3833</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I46" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C47" s="15" t="n">
         <v>1.6</v>
@@ -2682,21 +2773,21 @@
         <v>3833</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I47" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C48" s="15" t="n">
         <v>1.6</v>
@@ -2708,21 +2799,21 @@
         <v>3833</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I48" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C49" s="15" t="n">
         <v>1.6</v>
@@ -2734,125 +2825,125 @@
         <v>3833</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I49" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C50" s="15" t="n">
         <v>1.6</v>
       </c>
       <c r="D50" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E50" s="0" t="n">
         <v>3835</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="I50" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C51" s="15" t="n">
         <v>1.6</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E51" s="0" t="n">
         <v>2835</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="I51" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C52" s="15" t="n">
         <v>1.6</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E52" s="0" t="n">
         <v>3833</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="I52" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C53" s="15" t="n">
         <v>1.6</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E53" s="0" t="n">
         <v>2833</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="I53" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C54" s="15" t="n">
         <v>1.6</v>
@@ -2864,21 +2955,21 @@
         <v>3833</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I54" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C55" s="15" t="n">
         <v>1.6</v>
@@ -2890,21 +2981,21 @@
         <v>2833</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I55" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C56" s="15" t="n">
         <v>2.4</v>
@@ -2916,21 +3007,21 @@
         <v>3837</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="I56" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C57" s="15" t="n">
         <v>2.4</v>
@@ -2942,21 +3033,21 @@
         <v>2837</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H57" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="I57" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C58" s="15" t="n">
         <v>2.4</v>
@@ -2968,21 +3059,21 @@
         <v>3837</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="H58" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="I58" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C59" s="15" t="n">
         <v>2.4</v>
@@ -2994,21 +3085,21 @@
         <v>2837</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H59" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="I59" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C60" s="15" t="n">
         <v>2.4</v>
@@ -3020,21 +3111,21 @@
         <v>3837</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="H60" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="I60" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C61" s="15" t="n">
         <v>2.4</v>
@@ -3046,73 +3137,73 @@
         <v>2837</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H61" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="I61" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C62" s="15" t="n">
         <v>2.4</v>
       </c>
       <c r="D62" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E62" s="0" t="n">
         <v>3837</v>
       </c>
       <c r="G62" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="H62" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="I62" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C63" s="15" t="n">
         <v>2.4</v>
       </c>
       <c r="D63" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E63" s="0" t="n">
         <v>2837</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H63" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="I63" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C64" s="15" t="n">
         <v>2.4</v>
@@ -3124,21 +3215,21 @@
         <v>3837</v>
       </c>
       <c r="G64" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="H64" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I64" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C65" s="15" t="n">
         <v>2.4</v>
@@ -3150,73 +3241,73 @@
         <v>2837</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H65" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I65" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C66" s="15" t="n">
         <v>3</v>
       </c>
       <c r="D66" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E66" s="0" t="n">
         <v>3839</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="H66" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I66" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C67" s="15" t="n">
         <v>3</v>
       </c>
       <c r="D67" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E67" s="0" t="n">
         <v>2839</v>
       </c>
       <c r="G67" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="H67" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I67" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C68" s="15" t="n">
         <v>3</v>
@@ -3228,21 +3319,21 @@
         <v>3839</v>
       </c>
       <c r="G68" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="H68" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="I68" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C69" s="15" t="n">
         <v>3</v>
@@ -3254,21 +3345,21 @@
         <v>2839</v>
       </c>
       <c r="G69" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="H69" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="I69" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C70" s="15" t="n">
         <v>3</v>
@@ -3280,21 +3371,21 @@
         <v>3839</v>
       </c>
       <c r="G70" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="H70" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="I70" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C71" s="15" t="n">
         <v>3</v>
@@ -3306,21 +3397,21 @@
         <v>2839</v>
       </c>
       <c r="G71" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="H71" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="I71" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C72" s="15" t="n">
         <v>3</v>
@@ -3332,21 +3423,21 @@
         <v>3839</v>
       </c>
       <c r="G72" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H72" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="I72" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C73" s="15" t="n">
         <v>3</v>
@@ -3358,21 +3449,21 @@
         <v>2839</v>
       </c>
       <c r="G73" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="H73" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="I73" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C74" s="15" t="n">
         <v>4</v>
@@ -3384,21 +3475,21 @@
         <v>3841</v>
       </c>
       <c r="G74" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H74" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="I74" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C75" s="15" t="n">
         <v>4</v>
@@ -3410,73 +3501,73 @@
         <v>2841</v>
       </c>
       <c r="G75" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="H75" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="I75" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C76" s="15" t="n">
         <v>4</v>
       </c>
       <c r="D76" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E76" s="0" t="n">
         <v>3841</v>
       </c>
       <c r="G76" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H76" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="I76" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C77" s="15" t="n">
         <v>4</v>
       </c>
       <c r="D77" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E77" s="0" t="n">
         <v>2841</v>
       </c>
       <c r="G77" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="H77" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="I77" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C78" s="15" t="n">
         <v>4</v>
@@ -3488,21 +3579,21 @@
         <v>3841</v>
       </c>
       <c r="G78" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H78" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="I78" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C79" s="15" t="n">
         <v>4</v>
@@ -3514,73 +3605,73 @@
         <v>2841</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="H79" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="I79" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C80" s="15" t="n">
         <v>5</v>
       </c>
       <c r="D80" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E80" s="0" t="n">
         <v>3843</v>
       </c>
       <c r="G80" s="0" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="H80" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I80" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C81" s="15" t="n">
         <v>5</v>
       </c>
       <c r="D81" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E81" s="0" t="n">
         <v>2843</v>
       </c>
       <c r="G81" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="H81" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I81" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C82" s="15" t="n">
         <v>5</v>
@@ -3592,21 +3683,21 @@
         <v>3843</v>
       </c>
       <c r="G82" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="H82" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="I82" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C83" s="15" t="n">
         <v>5</v>
@@ -3618,99 +3709,99 @@
         <v>2843</v>
       </c>
       <c r="G83" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="H83" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="I83" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C84" s="15" t="n">
         <v>7</v>
       </c>
       <c r="D84" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E84" s="0" t="n">
         <v>3845</v>
       </c>
       <c r="G84" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="H84" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I84" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C85" s="15" t="n">
         <v>7</v>
       </c>
       <c r="D85" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E85" s="0" t="n">
         <v>2845</v>
       </c>
       <c r="G85" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="H85" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I85" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C86" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D86" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E86" s="0" t="n">
         <v>1831</v>
       </c>
       <c r="G86" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="H86" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I86" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C87" s="15" t="n">
         <v>0</v>
@@ -3722,47 +3813,47 @@
         <v>1831</v>
       </c>
       <c r="G87" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="H87" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I87" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C88" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D88" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E88" s="0" t="n">
         <v>1828</v>
       </c>
       <c r="G88" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="H88" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I88" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C89" s="15" t="n">
         <v>0</v>
@@ -3774,21 +3865,21 @@
         <v>1828</v>
       </c>
       <c r="G89" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="H89" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I89" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C90" s="15" t="n">
         <v>0</v>
@@ -3800,21 +3891,21 @@
         <v>1828</v>
       </c>
       <c r="G90" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="H90" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I90" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C91" s="15" t="n">
         <v>0</v>
@@ -3826,21 +3917,21 @@
         <v>1828</v>
       </c>
       <c r="G91" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="H91" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I91" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C92" s="15" t="n">
         <v>0</v>
@@ -3852,21 +3943,21 @@
         <v>1828</v>
       </c>
       <c r="G92" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="H92" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I92" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C93" s="15" t="n">
         <v>0</v>
@@ -3878,21 +3969,21 @@
         <v>1828</v>
       </c>
       <c r="G93" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="H93" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I93" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C94" s="15" t="n">
         <v>0</v>
@@ -3904,13 +3995,13 @@
         <v>1828</v>
       </c>
       <c r="G94" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="H94" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I94" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -3937,9 +4028,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.1295546558704"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.3441295546559"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.9554655870445"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.663967611336"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.7732793522267"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.3846153846154"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -4011,9 +4102,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.1295546558704"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.3441295546559"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="84.4089068825911"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.663967611336"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.7732793522267"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="85.1578947368421"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -4085,9 +4176,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.1295546558704"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.3441295546559"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="77.0202429149798"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.663967611336"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.7732793522267"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="77.6599190283401"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -4159,8 +4250,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="39.2064777327935"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="173.534412955466"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="39.5263157894737"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="175.137651821862"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="5" width="9.4251012145749"/>
   </cols>
   <sheetData>
@@ -4220,8 +4311,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="50.5587044534413"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="33.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="50.9878542510121"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="34.17004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="5" width="9.4251012145749"/>
   </cols>
   <sheetData>
@@ -4281,9 +4372,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.9878542510121"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.3076923076923"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.5991902834008"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.5222672064777"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.8461538461538"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.919028340081"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -4349,14 +4440,14 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="39.8502024291498"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="155.748987854251"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="40.17004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="157.141700404858"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="5" width="9.4251012145749"/>
   </cols>
   <sheetData>
@@ -4416,8 +4507,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="51.417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="79.3765182186235"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="51.8461538461539"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="80.0161943319838"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="5" width="9.4251012145749"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
PROS-5586 - MARSRU templates update
</commit_message>
<xml_diff>
--- a/Projects/MARSRU_PROD/Data/MARS must-range targets.xlsx
+++ b/Projects/MARSRU_PROD/Data/MARS must-range targets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="1648" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="114">
   <si>
     <t xml:space="preserve">Store type</t>
   </si>
@@ -476,175 +476,133 @@
     <t xml:space="preserve">4607065001063/5998749123072/4607065001025/5998749123058/4607065004514/4607065004446/5998749106877/5998749104392/5998749108147</t>
   </si>
   <si>
-    <t xml:space="preserve">Grocery Магазин у дома (&lt;100),
-Grocery Магазин у дома (100-299),
-Grocery Магазин у дома (300-449),
-Grocery Магазин у дома (450-599),
-Grocery Магазин у дома (600-999)
-Grocery Дискаунтер (&lt;300),
-Grocery Дискаунтер (300-999)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4607065377984,
-4607065001612,
-5998749106877,
-4607065001063,
-5000159438735
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grocery Магазин у дома (&lt;100),
-Grocery Магазин у дома (100-299),
-Grocery Магазин у дома (300-449),
-Grocery Магазин у дома (450-599),
-Grocery Магазин у дома (600-999)
-Grocery Дискаунтер (&lt;300),
-Grocery Дискаунтер (300-999),
-Grocery BIG BOXES (1000-2499),
-Grocery BIG BOXES (2500+)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4607065376048,
-4607065002862,
-4607065377984,
-4607065375119,
-5000159450881
-</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">4607065376048,
-4607065002862,
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">4607065371227,
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">4607065375119,
-4607065004071
-</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Grocery BIG BOXES (1000-2499),
-Grocery BIG BOXES (2500+)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">4607065377984
+    <t xml:space="preserve">KPI name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPI result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1834/1832/1836/1838/1840/1842/1844/2833/3833/3835/2835/3837/2837/3839/2839/3841/2841/3843/2843/3845/2845</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4607065377984
 4607065001612
 5998749106877
+4607065001063
+5000159438735</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4607065376048
+4607065002862
+4607065377984
+4607065375119
+5000159450881</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4607065376048
+4607065002862
+4607065371227
+4607065375119
+4607065004071</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1829/1826/1830/1827/1831/1828</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4607065377908
+4607065001612
+5998749106877
+4607065001063
+5000159438735</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4607065376048
+4607065002862
+4607065377908
+4607065375119
+5000159450881</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4607065003999
+4607065004019
+4607065004057
+4607065004118
+4607065375966
+4607065376000
+4607065376062
+4607065372057
+5000159373111
+5000159438698
+4011100157361
+4607065003838
+4607065374792
+5000159438674
+4607065374877
+4607065375034
+4607065378424
+4011100158399
+5000159438926
+5000159438940
+4607065371166
+4607065372217
+4607065372156
+4607065003944
+4607065002688</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4607065003999
+4607065004019
+4607065004057
+4607065004118
+4607065375966
+4607065376000
+4607065376062
+4607065372057
+5000159373111
+5000159438698
+4011100157361
+4607065003838
+4607065374792
+5000159438674
+4607065374877
+5000159451802
+4607065378424
+5000159425513
+5000159438926
+5000159438940
+4607065371166
+4607065372217
+4607065372156
+4607065003944
+4607065002541
 </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">5998749123072
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">5000159438735</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">4607065003999,
-4607065004019,
-4607065004057,
-4607065004118,
-4607065375966,
-4607065376000,
-4607065376062,
-4607065372057,
-5000159373111,
-5000159438698,
-4011100157361,
-4607065003838,
-4607065374792,
-5000159438674,
-4607065374877,
-4607065375034,
-4607065378424,
-4011100158399,
-5000159438926,
-5000159438940,
-4607065371166,
-4607065372217,
-4607065372156,
-4607065003944,
-4607065002688</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4607065003999,
-4607065004019,
-4607065004057,
-4607065004118,
-4607065375966,
-4607065376000,
-4607065376062,
-4607065372057,
-5000159373111,
-5000159438698,
-4011100157361,
-4607065003838,
-4607065374792,
-5000159438674,
-4607065374877,
-4607065375034,
-4607065378424,
-4011100158399,
-5000159438926,
-5000159438940,
-4607065371166,
-4607065372217,
-4607065372156,
-4607065003944,
-4607065002688
-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4607065003999
+4607065004019
+4607065004057
+4607065004118
+4607065375966
+4607065376000
+4607065376062
+4607065372057
+5000159373111
+5000159438698
+4011100157361
+4607065003838
+4607065374792
+5000159438674
+4607065374877
+5000159451802
+4607065378424
+5000159425513
+5000159438926
+5000159438940
+4607065371166
+4607065372217
+4607065372156
+4607065003944
+4607065002541</t>
   </si>
   <si>
     <t xml:space="preserve">Shelf # from the bottom</t>
@@ -874,7 +832,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -900,22 +858,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -979,7 +921,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1024,12 +966,16 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1125,7 +1071,7 @@
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF00B050"/>
+      <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -1150,9 +1096,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.4534412955466"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.8421052631579"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.5222672064777"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.7773279352227"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.3805668016194"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.0607287449393"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1260,73 +1206,117 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.3117408906883"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.5222672064777"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="84.4089068825911"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="64.0566801619433"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.64777327935223"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.7408906882591"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.8097165991903"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.4251012145749"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="94.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="10" t="s">
+    <row r="2" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="121.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
+      <c r="B2" s="11" t="n">
+        <v>2254</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="D2" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="121.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
+      <c r="B3" s="11" t="n">
+        <v>2254</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="D3" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="66.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
+      <c r="B4" s="11" t="n">
+        <v>2254</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="10" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="10" t="s">
         <v>4</v>
+      </c>
+      <c r="B5" s="11" t="n">
+        <v>2254</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>35</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="11" t="n">
+        <v>2254</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="11" t="n">
+        <v>2254</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1345,86 +1335,119 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.0607287449393"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.0242914979757"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="120.935222672065"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="56.4534412955466"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.11336032388664"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.4898785425101"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.3076923076923"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.4251012145749"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="356.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
+    <row r="2" customFormat="false" ht="355.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="11" t="n">
+        <v>2254</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="D2" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="337.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="11" t="n">
+        <v>2254</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="337.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="11" t="n">
+        <v>2254</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="350.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="350.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="B5" s="11" t="n">
+        <v>2254</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="337.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="350.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="B6" s="11" t="n">
+        <v>2254</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="337.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="B7" s="11" t="n">
+        <v>2254</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1449,89 +1472,89 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.5991902834008"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.919028340081"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.1740890688259"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>38</v>
+      <c r="B1" s="14" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14" t="s">
-        <v>39</v>
+      <c r="A2" s="15" t="s">
+        <v>42</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="14" t="s">
-        <v>41</v>
+      <c r="A3" s="15" t="s">
+        <v>44</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="14" t="s">
-        <v>42</v>
+      <c r="A4" s="15" t="s">
+        <v>45</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14" t="s">
-        <v>44</v>
+      <c r="A5" s="15" t="s">
+        <v>47</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="14" t="s">
-        <v>45</v>
+      <c r="A6" s="15" t="s">
+        <v>48</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14" t="s">
-        <v>47</v>
+      <c r="A8" s="15" t="s">
+        <v>50</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="14" t="s">
-        <v>48</v>
+      <c r="A9" s="15" t="s">
+        <v>51</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="14" t="s">
-        <v>49</v>
+      <c r="A10" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1558,2461 +1581,2461 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0647773279352"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.8137651821862"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="15" width="29.2429149797571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="15" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.0283400809717"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="16" width="29.4574898785425"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="16" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.5668016194332"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.53441295546559"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="43.3846153846154"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.1012145748988"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="43.7044534412956"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.0283400809717"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.4251012145749"/>
   </cols>
   <sheetData>
-    <row r="1" s="15" customFormat="true" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" s="16" t="s">
+    <row r="1" s="16" customFormat="true" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="D1" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="E1" s="17" t="s">
         <v>56</v>
       </c>
+      <c r="F1" s="18"/>
+      <c r="G1" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="20" t="s">
-        <v>57</v>
+      <c r="A2" s="21" t="s">
+        <v>60</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="15" t="n">
+        <v>47</v>
+      </c>
+      <c r="C2" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>58</v>
+      <c r="D2" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>1834</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="15" t="n">
+        <v>49</v>
+      </c>
+      <c r="C3" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="D3" s="15" t="s">
-        <v>58</v>
+      <c r="D3" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>1832</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="15" t="n">
+        <v>50</v>
+      </c>
+      <c r="C4" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="D4" s="15" t="n">
+      <c r="D4" s="16" t="n">
         <v>2.4</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>1832</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="15" t="n">
+        <v>50</v>
+      </c>
+      <c r="C5" s="16" t="n">
         <v>2.4</v>
       </c>
-      <c r="D5" s="15" t="s">
-        <v>58</v>
+      <c r="D5" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>1836</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="15" t="n">
+        <v>51</v>
+      </c>
+      <c r="C6" s="16" t="n">
         <v>2.4</v>
       </c>
-      <c r="D6" s="15" t="n">
+      <c r="D6" s="16" t="n">
         <v>3</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>1836</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="15" t="n">
+        <v>51</v>
+      </c>
+      <c r="C7" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="D7" s="15" t="s">
-        <v>58</v>
+      <c r="D7" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>1838</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="15" t="n">
+        <v>52</v>
+      </c>
+      <c r="C8" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="D8" s="15" t="n">
+      <c r="D8" s="16" t="n">
         <v>4</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>1838</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="15" t="n">
+        <v>42</v>
+      </c>
+      <c r="C9" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="D9" s="15" t="n">
+      <c r="D9" s="16" t="n">
         <v>4</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>1838</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="15" t="n">
+        <v>44</v>
+      </c>
+      <c r="C10" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="D10" s="15" t="n">
+      <c r="D10" s="16" t="n">
         <v>4</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>1838</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="15" t="n">
+        <v>42</v>
+      </c>
+      <c r="C11" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="D11" s="15" t="n">
+      <c r="D11" s="16" t="n">
         <v>5</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>1840</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="15" t="n">
+        <v>52</v>
+      </c>
+      <c r="C12" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="D12" s="15" t="s">
-        <v>58</v>
+      <c r="D12" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>1840</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="15" t="n">
+        <v>44</v>
+      </c>
+      <c r="C13" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="D13" s="15" t="n">
+      <c r="D13" s="16" t="n">
         <v>5</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>1840</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="15" t="n">
+        <v>42</v>
+      </c>
+      <c r="C14" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="D14" s="15" t="s">
-        <v>58</v>
+      <c r="D14" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>1842</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="15" t="n">
+        <v>44</v>
+      </c>
+      <c r="C15" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="D15" s="15" t="n">
+      <c r="D15" s="16" t="n">
         <v>7</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>1842</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>58</v>
+        <v>45</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>1829</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="15" t="n">
+        <v>47</v>
+      </c>
+      <c r="C17" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D17" s="15" t="n">
+      <c r="D17" s="16" t="n">
         <v>1.6</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>1829</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>58</v>
+        <v>48</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>1826</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="15" t="n">
+        <v>49</v>
+      </c>
+      <c r="C19" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D19" s="15" t="n">
+      <c r="D19" s="16" t="n">
         <v>1.6</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>1826</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="15" t="n">
+        <v>42</v>
+      </c>
+      <c r="C20" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D20" s="15" t="n">
+      <c r="D20" s="16" t="n">
         <v>1.6</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>1826</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="15" t="n">
+        <v>44</v>
+      </c>
+      <c r="C21" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D21" s="15" t="n">
+      <c r="D21" s="16" t="n">
         <v>1.6</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>1826</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="15" t="n">
+        <v>52</v>
+      </c>
+      <c r="C22" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D22" s="15" t="n">
+      <c r="D22" s="16" t="n">
         <v>1.6</v>
       </c>
       <c r="E22" s="0" t="n">
         <v>1826</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="15" t="n">
+        <v>51</v>
+      </c>
+      <c r="C23" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D23" s="15" t="n">
+      <c r="D23" s="16" t="n">
         <v>1.6</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>1826</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="15" t="n">
+        <v>50</v>
+      </c>
+      <c r="C24" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D24" s="15" t="n">
+      <c r="D24" s="16" t="n">
         <v>1.6</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>1826</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="15" t="n">
+        <v>44</v>
+      </c>
+      <c r="C25" s="16" t="n">
         <v>7</v>
       </c>
-      <c r="D25" s="15" t="s">
-        <v>58</v>
+      <c r="D25" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>1844</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" s="15" t="n">
+        <v>42</v>
+      </c>
+      <c r="C26" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="D26" s="15" t="n">
+      <c r="D26" s="16" t="n">
         <v>2.4</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>1832</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="15" t="n">
+        <v>44</v>
+      </c>
+      <c r="C27" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="D27" s="15" t="n">
+      <c r="D27" s="16" t="n">
         <v>2.4</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>1832</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" s="15" t="n">
+        <v>52</v>
+      </c>
+      <c r="C28" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="D28" s="15" t="n">
+      <c r="D28" s="16" t="n">
         <v>2.4</v>
       </c>
       <c r="E28" s="0" t="n">
         <v>1832</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C29" s="15" t="n">
+        <v>51</v>
+      </c>
+      <c r="C29" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="D29" s="15" t="n">
+      <c r="D29" s="16" t="n">
         <v>2.4</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>1832</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C30" s="15" t="n">
+        <v>42</v>
+      </c>
+      <c r="C30" s="16" t="n">
         <v>2.4</v>
       </c>
-      <c r="D30" s="15" t="n">
+      <c r="D30" s="16" t="n">
         <v>3</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>1836</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C31" s="15" t="n">
+        <v>44</v>
+      </c>
+      <c r="C31" s="16" t="n">
         <v>2.4</v>
       </c>
-      <c r="D31" s="15" t="n">
+      <c r="D31" s="16" t="n">
         <v>3</v>
       </c>
       <c r="E31" s="0" t="n">
         <v>1836</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32" s="15" t="n">
+        <v>52</v>
+      </c>
+      <c r="C32" s="16" t="n">
         <v>2.4</v>
       </c>
-      <c r="D32" s="15" t="n">
+      <c r="D32" s="16" t="n">
         <v>3</v>
       </c>
       <c r="E32" s="0" t="n">
         <v>1836</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>58</v>
+        <v>45</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="E33" s="0" t="n">
         <v>1830</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="C34" s="15" t="n">
+        <v>47</v>
+      </c>
+      <c r="C34" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D34" s="15" t="n">
+      <c r="D34" s="16" t="n">
         <v>1.6</v>
       </c>
       <c r="E34" s="0" t="n">
         <v>1830</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D35" s="15" t="s">
-        <v>58</v>
+        <v>48</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="E35" s="0" t="n">
         <v>1827</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C36" s="15" t="n">
+        <v>49</v>
+      </c>
+      <c r="C36" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D36" s="15" t="n">
+      <c r="D36" s="16" t="n">
         <v>1.6</v>
       </c>
       <c r="E36" s="0" t="n">
         <v>1827</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C37" s="15" t="n">
+        <v>42</v>
+      </c>
+      <c r="C37" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D37" s="15" t="n">
+      <c r="D37" s="16" t="n">
         <v>1.6</v>
       </c>
       <c r="E37" s="0" t="n">
         <v>1827</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C38" s="15" t="n">
+        <v>44</v>
+      </c>
+      <c r="C38" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D38" s="15" t="n">
+      <c r="D38" s="16" t="n">
         <v>1.6</v>
       </c>
       <c r="E38" s="0" t="n">
         <v>1827</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I38" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C39" s="15" t="n">
+        <v>52</v>
+      </c>
+      <c r="C39" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D39" s="15" t="n">
+      <c r="D39" s="16" t="n">
         <v>1.6</v>
       </c>
       <c r="E39" s="0" t="n">
         <v>1827</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I39" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C40" s="15" t="n">
+        <v>51</v>
+      </c>
+      <c r="C40" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D40" s="15" t="n">
+      <c r="D40" s="16" t="n">
         <v>1.6</v>
       </c>
       <c r="E40" s="0" t="n">
         <v>1827</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I40" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="C41" s="15" t="n">
+        <v>50</v>
+      </c>
+      <c r="C41" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D41" s="15" t="n">
+      <c r="D41" s="16" t="n">
         <v>1.6</v>
       </c>
       <c r="E41" s="0" t="n">
         <v>1827</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I41" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C42" s="15" t="n">
+        <v>42</v>
+      </c>
+      <c r="C42" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="D42" s="15" t="n">
+      <c r="D42" s="16" t="n">
         <v>2.4</v>
       </c>
       <c r="E42" s="0" t="n">
         <v>2833</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I42" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C43" s="15" t="n">
+        <v>44</v>
+      </c>
+      <c r="C43" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="D43" s="15" t="n">
+      <c r="D43" s="16" t="n">
         <v>2.4</v>
       </c>
       <c r="E43" s="0" t="n">
         <v>2833</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I43" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C44" s="15" t="n">
+        <v>52</v>
+      </c>
+      <c r="C44" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="D44" s="15" t="n">
+      <c r="D44" s="16" t="n">
         <v>2.4</v>
       </c>
       <c r="E44" s="0" t="n">
         <v>2833</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I44" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C45" s="15" t="n">
+        <v>51</v>
+      </c>
+      <c r="C45" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="D45" s="15" t="n">
+      <c r="D45" s="16" t="n">
         <v>2.4</v>
       </c>
       <c r="E45" s="0" t="n">
         <v>2833</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I45" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C46" s="15" t="n">
+        <v>42</v>
+      </c>
+      <c r="C46" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="D46" s="15" t="n">
+      <c r="D46" s="16" t="n">
         <v>2.4</v>
       </c>
       <c r="E46" s="0" t="n">
         <v>3833</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I46" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C47" s="15" t="n">
+        <v>44</v>
+      </c>
+      <c r="C47" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="D47" s="15" t="n">
+      <c r="D47" s="16" t="n">
         <v>2.4</v>
       </c>
       <c r="E47" s="0" t="n">
         <v>3833</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I47" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C48" s="15" t="n">
+        <v>52</v>
+      </c>
+      <c r="C48" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="D48" s="15" t="n">
+      <c r="D48" s="16" t="n">
         <v>2.4</v>
       </c>
       <c r="E48" s="0" t="n">
         <v>3833</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I48" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C49" s="15" t="n">
+        <v>51</v>
+      </c>
+      <c r="C49" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="D49" s="15" t="n">
+      <c r="D49" s="16" t="n">
         <v>2.4</v>
       </c>
       <c r="E49" s="0" t="n">
         <v>3833</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I49" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="C50" s="15" t="n">
+        <v>47</v>
+      </c>
+      <c r="C50" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="D50" s="15" t="s">
-        <v>58</v>
+      <c r="D50" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="E50" s="0" t="n">
         <v>3835</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I50" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="C51" s="15" t="n">
+        <v>47</v>
+      </c>
+      <c r="C51" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="D51" s="15" t="s">
-        <v>58</v>
+      <c r="D51" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="E51" s="0" t="n">
         <v>2835</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I51" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C52" s="15" t="n">
+        <v>49</v>
+      </c>
+      <c r="C52" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="D52" s="15" t="s">
-        <v>58</v>
+      <c r="D52" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="E52" s="0" t="n">
         <v>3833</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I52" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C53" s="15" t="n">
+        <v>49</v>
+      </c>
+      <c r="C53" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="D53" s="15" t="s">
-        <v>58</v>
+      <c r="D53" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="E53" s="0" t="n">
         <v>2833</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I53" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="C54" s="15" t="n">
+        <v>50</v>
+      </c>
+      <c r="C54" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="D54" s="15" t="n">
+      <c r="D54" s="16" t="n">
         <v>2.4</v>
       </c>
       <c r="E54" s="0" t="n">
         <v>3833</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I54" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="C55" s="15" t="n">
+        <v>50</v>
+      </c>
+      <c r="C55" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="D55" s="15" t="n">
+      <c r="D55" s="16" t="n">
         <v>2.4</v>
       </c>
       <c r="E55" s="0" t="n">
         <v>2833</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I55" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C56" s="15" t="n">
+        <v>42</v>
+      </c>
+      <c r="C56" s="16" t="n">
         <v>2.4</v>
       </c>
-      <c r="D56" s="15" t="n">
+      <c r="D56" s="16" t="n">
         <v>3</v>
       </c>
       <c r="E56" s="0" t="n">
         <v>3837</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="I56" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C57" s="15" t="n">
+        <v>42</v>
+      </c>
+      <c r="C57" s="16" t="n">
         <v>2.4</v>
       </c>
-      <c r="D57" s="15" t="n">
+      <c r="D57" s="16" t="n">
         <v>3</v>
       </c>
       <c r="E57" s="0" t="n">
         <v>2837</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="H57" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="I57" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C58" s="15" t="n">
+        <v>44</v>
+      </c>
+      <c r="C58" s="16" t="n">
         <v>2.4</v>
       </c>
-      <c r="D58" s="15" t="n">
+      <c r="D58" s="16" t="n">
         <v>3</v>
       </c>
       <c r="E58" s="0" t="n">
         <v>3837</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H58" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="I58" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C59" s="15" t="n">
+        <v>44</v>
+      </c>
+      <c r="C59" s="16" t="n">
         <v>2.4</v>
       </c>
-      <c r="D59" s="15" t="n">
+      <c r="D59" s="16" t="n">
         <v>3</v>
       </c>
       <c r="E59" s="0" t="n">
         <v>2837</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="H59" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="I59" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C60" s="15" t="n">
+        <v>52</v>
+      </c>
+      <c r="C60" s="16" t="n">
         <v>2.4</v>
       </c>
-      <c r="D60" s="15" t="n">
+      <c r="D60" s="16" t="n">
         <v>3</v>
       </c>
       <c r="E60" s="0" t="n">
         <v>3837</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H60" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="I60" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C61" s="15" t="n">
+        <v>52</v>
+      </c>
+      <c r="C61" s="16" t="n">
         <v>2.4</v>
       </c>
-      <c r="D61" s="15" t="n">
+      <c r="D61" s="16" t="n">
         <v>3</v>
       </c>
       <c r="E61" s="0" t="n">
         <v>2837</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="H61" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="I61" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="C62" s="15" t="n">
+        <v>50</v>
+      </c>
+      <c r="C62" s="16" t="n">
         <v>2.4</v>
       </c>
-      <c r="D62" s="15" t="s">
-        <v>58</v>
+      <c r="D62" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="E62" s="0" t="n">
         <v>3837</v>
       </c>
       <c r="G62" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="H62" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I62" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="C63" s="15" t="n">
+        <v>50</v>
+      </c>
+      <c r="C63" s="16" t="n">
         <v>2.4</v>
       </c>
-      <c r="D63" s="15" t="s">
-        <v>58</v>
+      <c r="D63" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="E63" s="0" t="n">
         <v>2837</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="H63" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I63" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C64" s="15" t="n">
+        <v>51</v>
+      </c>
+      <c r="C64" s="16" t="n">
         <v>2.4</v>
       </c>
-      <c r="D64" s="15" t="n">
+      <c r="D64" s="16" t="n">
         <v>3</v>
       </c>
       <c r="E64" s="0" t="n">
         <v>3837</v>
       </c>
       <c r="G64" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H64" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="I64" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C65" s="15" t="n">
+        <v>51</v>
+      </c>
+      <c r="C65" s="16" t="n">
         <v>2.4</v>
       </c>
-      <c r="D65" s="15" t="n">
+      <c r="D65" s="16" t="n">
         <v>3</v>
       </c>
       <c r="E65" s="0" t="n">
         <v>2837</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="H65" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="I65" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C66" s="15" t="n">
+        <v>51</v>
+      </c>
+      <c r="C66" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="D66" s="15" t="s">
-        <v>58</v>
+      <c r="D66" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="E66" s="0" t="n">
         <v>3839</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H66" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="I66" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C67" s="15" t="n">
+        <v>51</v>
+      </c>
+      <c r="C67" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="D67" s="15" t="s">
-        <v>58</v>
+      <c r="D67" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="E67" s="0" t="n">
         <v>2839</v>
       </c>
       <c r="G67" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="H67" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="I67" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C68" s="15" t="n">
+        <v>52</v>
+      </c>
+      <c r="C68" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="D68" s="15" t="n">
+      <c r="D68" s="16" t="n">
         <v>4</v>
       </c>
       <c r="E68" s="0" t="n">
         <v>3839</v>
       </c>
       <c r="G68" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H68" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="I68" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C69" s="15" t="n">
+        <v>52</v>
+      </c>
+      <c r="C69" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="D69" s="15" t="n">
+      <c r="D69" s="16" t="n">
         <v>4</v>
       </c>
       <c r="E69" s="0" t="n">
         <v>2839</v>
       </c>
       <c r="G69" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="H69" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="I69" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C70" s="15" t="n">
+        <v>42</v>
+      </c>
+      <c r="C70" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="D70" s="15" t="n">
+      <c r="D70" s="16" t="n">
         <v>4</v>
       </c>
       <c r="E70" s="0" t="n">
         <v>3839</v>
       </c>
       <c r="G70" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H70" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="I70" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C71" s="15" t="n">
+        <v>42</v>
+      </c>
+      <c r="C71" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="D71" s="15" t="n">
+      <c r="D71" s="16" t="n">
         <v>4</v>
       </c>
       <c r="E71" s="0" t="n">
         <v>2839</v>
       </c>
       <c r="G71" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="H71" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="I71" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C72" s="15" t="n">
+        <v>44</v>
+      </c>
+      <c r="C72" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="D72" s="15" t="n">
+      <c r="D72" s="16" t="n">
         <v>4</v>
       </c>
       <c r="E72" s="0" t="n">
         <v>3839</v>
       </c>
       <c r="G72" s="0" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="H72" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="I72" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C73" s="15" t="n">
+        <v>44</v>
+      </c>
+      <c r="C73" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="D73" s="15" t="n">
+      <c r="D73" s="16" t="n">
         <v>4</v>
       </c>
       <c r="E73" s="0" t="n">
         <v>2839</v>
       </c>
       <c r="G73" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="H73" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="I73" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C74" s="15" t="n">
+        <v>42</v>
+      </c>
+      <c r="C74" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="D74" s="15" t="n">
+      <c r="D74" s="16" t="n">
         <v>5</v>
       </c>
       <c r="E74" s="0" t="n">
         <v>3841</v>
       </c>
       <c r="G74" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="H74" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I74" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C75" s="15" t="n">
+        <v>42</v>
+      </c>
+      <c r="C75" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="D75" s="15" t="n">
+      <c r="D75" s="16" t="n">
         <v>5</v>
       </c>
       <c r="E75" s="0" t="n">
         <v>2841</v>
       </c>
       <c r="G75" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="H75" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I75" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C76" s="15" t="n">
+        <v>52</v>
+      </c>
+      <c r="C76" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="D76" s="15" t="s">
-        <v>58</v>
+      <c r="D76" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="E76" s="0" t="n">
         <v>3841</v>
       </c>
       <c r="G76" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="H76" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="I76" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C77" s="15" t="n">
+        <v>52</v>
+      </c>
+      <c r="C77" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="D77" s="15" t="s">
-        <v>58</v>
+      <c r="D77" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="E77" s="0" t="n">
         <v>2841</v>
       </c>
       <c r="G77" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="H77" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="I77" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C78" s="15" t="n">
+        <v>44</v>
+      </c>
+      <c r="C78" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="D78" s="15" t="n">
+      <c r="D78" s="16" t="n">
         <v>5</v>
       </c>
       <c r="E78" s="0" t="n">
         <v>3841</v>
       </c>
       <c r="G78" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="H78" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I78" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C79" s="15" t="n">
+        <v>44</v>
+      </c>
+      <c r="C79" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="D79" s="15" t="n">
+      <c r="D79" s="16" t="n">
         <v>5</v>
       </c>
       <c r="E79" s="0" t="n">
         <v>2841</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="H79" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I79" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C80" s="15" t="n">
+        <v>42</v>
+      </c>
+      <c r="C80" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="D80" s="15" t="s">
-        <v>58</v>
+      <c r="D80" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="E80" s="0" t="n">
         <v>3843</v>
       </c>
       <c r="G80" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="H80" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I80" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C81" s="15" t="n">
+        <v>42</v>
+      </c>
+      <c r="C81" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="D81" s="15" t="s">
-        <v>58</v>
+      <c r="D81" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="E81" s="0" t="n">
         <v>2843</v>
       </c>
       <c r="G81" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="H81" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I81" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C82" s="15" t="n">
+        <v>44</v>
+      </c>
+      <c r="C82" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="D82" s="15" t="n">
+      <c r="D82" s="16" t="n">
         <v>7</v>
       </c>
       <c r="E82" s="0" t="n">
         <v>3843</v>
       </c>
       <c r="G82" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="H82" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I82" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C83" s="15" t="n">
+        <v>44</v>
+      </c>
+      <c r="C83" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="D83" s="15" t="n">
+      <c r="D83" s="16" t="n">
         <v>7</v>
       </c>
       <c r="E83" s="0" t="n">
         <v>2843</v>
       </c>
       <c r="G83" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="H83" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I83" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C84" s="15" t="n">
+        <v>44</v>
+      </c>
+      <c r="C84" s="16" t="n">
         <v>7</v>
       </c>
-      <c r="D84" s="15" t="s">
-        <v>58</v>
+      <c r="D84" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="E84" s="0" t="n">
         <v>3845</v>
       </c>
       <c r="G84" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="H84" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="I84" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C85" s="15" t="n">
+        <v>44</v>
+      </c>
+      <c r="C85" s="16" t="n">
         <v>7</v>
       </c>
-      <c r="D85" s="15" t="s">
-        <v>58</v>
+      <c r="D85" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="E85" s="0" t="n">
         <v>2845</v>
       </c>
       <c r="G85" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="H85" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="I85" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="C86" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D86" s="15" t="s">
-        <v>58</v>
+        <v>45</v>
+      </c>
+      <c r="C86" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D86" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="E86" s="0" t="n">
         <v>1831</v>
       </c>
       <c r="G86" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="H86" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="I86" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="C87" s="15" t="n">
+        <v>47</v>
+      </c>
+      <c r="C87" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D87" s="15" t="n">
+      <c r="D87" s="16" t="n">
         <v>1.6</v>
       </c>
       <c r="E87" s="0" t="n">
         <v>1831</v>
       </c>
       <c r="G87" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="H87" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I87" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C88" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D88" s="15" t="s">
-        <v>58</v>
+        <v>48</v>
+      </c>
+      <c r="C88" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D88" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="E88" s="0" t="n">
         <v>1828</v>
       </c>
       <c r="G88" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="H88" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="I88" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C89" s="15" t="n">
+        <v>49</v>
+      </c>
+      <c r="C89" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D89" s="15" t="n">
+      <c r="D89" s="16" t="n">
         <v>1.6</v>
       </c>
       <c r="E89" s="0" t="n">
         <v>1828</v>
       </c>
       <c r="G89" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="H89" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I89" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C90" s="15" t="n">
+        <v>42</v>
+      </c>
+      <c r="C90" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D90" s="15" t="n">
+      <c r="D90" s="16" t="n">
         <v>1.6</v>
       </c>
       <c r="E90" s="0" t="n">
         <v>1828</v>
       </c>
       <c r="G90" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="H90" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I90" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C91" s="15" t="n">
+        <v>44</v>
+      </c>
+      <c r="C91" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D91" s="15" t="n">
+      <c r="D91" s="16" t="n">
         <v>1.6</v>
       </c>
       <c r="E91" s="0" t="n">
         <v>1828</v>
       </c>
       <c r="G91" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="H91" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I91" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C92" s="15" t="n">
+        <v>52</v>
+      </c>
+      <c r="C92" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D92" s="15" t="n">
+      <c r="D92" s="16" t="n">
         <v>1.6</v>
       </c>
       <c r="E92" s="0" t="n">
         <v>1828</v>
       </c>
       <c r="G92" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="H92" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I92" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C93" s="15" t="n">
+        <v>51</v>
+      </c>
+      <c r="C93" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D93" s="15" t="n">
+      <c r="D93" s="16" t="n">
         <v>1.6</v>
       </c>
       <c r="E93" s="0" t="n">
         <v>1828</v>
       </c>
       <c r="G93" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="H93" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I93" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="C94" s="15" t="n">
+        <v>50</v>
+      </c>
+      <c r="C94" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D94" s="15" t="n">
+      <c r="D94" s="16" t="n">
         <v>1.6</v>
       </c>
       <c r="E94" s="0" t="n">
         <v>1828</v>
       </c>
       <c r="G94" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="H94" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I94" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -4039,9 +4062,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.1983805668016"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.3076923076923"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.7044534412956"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.7368421052632"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.8461538461538"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.0242914979757"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -4113,9 +4136,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.1983805668016"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.3076923076923"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="85.9109311740891"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.7368421052632"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.8461538461538"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.6599190283401"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -4187,9 +4210,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.1983805668016"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.3076923076923"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="78.3036437246964"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.7368421052632"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.8461538461538"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.0526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -4261,8 +4284,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="39.8502024291498"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="176.744939271255"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="40.17004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="178.352226720648"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="5" width="9.4251012145749"/>
   </cols>
   <sheetData>
@@ -4322,8 +4345,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="51.417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="34.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="51.8461538461539"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="34.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="5" width="9.4251012145749"/>
   </cols>
   <sheetData>
@@ -4383,9 +4406,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="64.0566801619433"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.3805668016194"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.2388663967611"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="64.7004048582996"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.8097165991903"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.5627530364373"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -4452,13 +4475,13 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="40.5991902834008"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="158.534412955466"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="40.919028340081"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="126.878542510121"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="5" width="9.4251012145749"/>
   </cols>
   <sheetData>
@@ -4518,8 +4541,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="52.2753036437247"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="80.6599190283401"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="52.7044534412956"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="81.4089068825911"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="5" width="9.4251012145749"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
PROS-5586 - MARSRU - kpi update
</commit_message>
<xml_diff>
--- a/Projects/MARSRU_PROD/Data/MARS must-range targets.xlsx
+++ b/Projects/MARSRU_PROD/Data/MARS must-range targets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="1648" sheetId="1" state="visible" r:id="rId2"/>
@@ -921,7 +921,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -994,16 +994,8 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1096,9 +1088,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.7773279352227"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.3805668016194"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.0607287449393"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.0971659919028"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.8056680161943"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.5951417004049"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1209,15 +1201,15 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="64.0566801619433"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.64777327935223"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.7408906882591"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.8097165991903"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1821862348178"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.67611336032389"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.165991902834"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.8906882591093"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.4251012145749"/>
   </cols>
   <sheetData>
@@ -1343,10 +1335,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="56.4534412955466"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.11336032388664"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.4898785425101"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.3076923076923"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1821862348178"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.8097165991903"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5303643724696"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.4251012145749"/>
   </cols>
   <sheetData>
@@ -1472,8 +1464,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.1740890688259"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.2388663967611"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.3846153846154"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1573,24 +1565,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I94"/>
+  <dimension ref="1:94"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.0283400809717"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="16" width="29.4574898785425"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="16" width="27.2064777327935"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.53441295546559"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="43.7044534412956"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.2105263157895"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.0971659919028"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.3481781376518"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="16" width="29.6720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="16" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="16" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.0242914979757"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.4251012145749"/>
   </cols>
   <sheetData>
     <row r="1" s="16" customFormat="true" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1609,19 +1600,19 @@
       <c r="E1" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="18"/>
-      <c r="G1" s="19" t="s">
+      <c r="F1" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="G1" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="H1" s="18" t="s">
         <v>59</v>
       </c>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="19" t="s">
         <v>60</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -1633,16 +1624,16 @@
       <c r="D2" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="16" t="n">
         <v>1834</v>
       </c>
+      <c r="F2" s="0" t="s">
+        <v>62</v>
+      </c>
       <c r="G2" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="I2" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1659,16 +1650,16 @@
       <c r="D3" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="16" t="n">
         <v>1832</v>
       </c>
+      <c r="F3" s="0" t="s">
+        <v>65</v>
+      </c>
       <c r="G3" s="0" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="I3" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1685,16 +1676,16 @@
       <c r="D4" s="16" t="n">
         <v>2.4</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="16" t="n">
         <v>1832</v>
       </c>
+      <c r="F4" s="0" t="s">
+        <v>65</v>
+      </c>
       <c r="G4" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="I4" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1711,16 +1702,16 @@
       <c r="D5" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="16" t="n">
         <v>1836</v>
       </c>
+      <c r="F5" s="0" t="s">
+        <v>67</v>
+      </c>
       <c r="G5" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="I5" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1737,16 +1728,16 @@
       <c r="D6" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="16" t="n">
         <v>1836</v>
       </c>
+      <c r="F6" s="0" t="s">
+        <v>67</v>
+      </c>
       <c r="G6" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="I6" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1763,16 +1754,16 @@
       <c r="D7" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="16" t="n">
         <v>1838</v>
       </c>
+      <c r="F7" s="0" t="s">
+        <v>70</v>
+      </c>
       <c r="G7" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="I7" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1789,16 +1780,16 @@
       <c r="D8" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="16" t="n">
         <v>1838</v>
       </c>
+      <c r="F8" s="0" t="s">
+        <v>70</v>
+      </c>
       <c r="G8" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="I8" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1815,16 +1806,16 @@
       <c r="D9" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="16" t="n">
         <v>1838</v>
       </c>
+      <c r="F9" s="0" t="s">
+        <v>70</v>
+      </c>
       <c r="G9" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="I9" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1841,16 +1832,16 @@
       <c r="D10" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="16" t="n">
         <v>1838</v>
       </c>
+      <c r="F10" s="0" t="s">
+        <v>70</v>
+      </c>
       <c r="G10" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="I10" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1867,16 +1858,16 @@
       <c r="D11" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="16" t="n">
         <v>1840</v>
       </c>
+      <c r="F11" s="0" t="s">
+        <v>73</v>
+      </c>
       <c r="G11" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="I11" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1893,16 +1884,16 @@
       <c r="D12" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="16" t="n">
         <v>1840</v>
       </c>
+      <c r="F12" s="0" t="s">
+        <v>73</v>
+      </c>
       <c r="G12" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="I12" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1919,16 +1910,16 @@
       <c r="D13" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="16" t="n">
         <v>1840</v>
       </c>
+      <c r="F13" s="0" t="s">
+        <v>73</v>
+      </c>
       <c r="G13" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="I13" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1945,16 +1936,16 @@
       <c r="D14" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="16" t="n">
         <v>1842</v>
       </c>
+      <c r="F14" s="0" t="s">
+        <v>76</v>
+      </c>
       <c r="G14" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="I14" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1971,16 +1962,16 @@
       <c r="D15" s="16" t="n">
         <v>7</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="16" t="n">
         <v>1842</v>
       </c>
+      <c r="F15" s="0" t="s">
+        <v>76</v>
+      </c>
       <c r="G15" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="I15" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1997,16 +1988,16 @@
       <c r="D16" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="16" t="n">
         <v>1829</v>
       </c>
+      <c r="F16" s="0" t="s">
+        <v>79</v>
+      </c>
       <c r="G16" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="I16" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2023,16 +2014,16 @@
       <c r="D17" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="16" t="n">
         <v>1829</v>
       </c>
+      <c r="F17" s="0" t="s">
+        <v>79</v>
+      </c>
       <c r="G17" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="I17" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2049,16 +2040,16 @@
       <c r="D18" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="16" t="n">
         <v>1826</v>
       </c>
+      <c r="F18" s="0" t="s">
+        <v>82</v>
+      </c>
       <c r="G18" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="I18" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2075,16 +2066,16 @@
       <c r="D19" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19" s="16" t="n">
         <v>1826</v>
       </c>
+      <c r="F19" s="0" t="s">
+        <v>82</v>
+      </c>
       <c r="G19" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="I19" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2101,16 +2092,16 @@
       <c r="D20" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="E20" s="0" t="n">
+      <c r="E20" s="16" t="n">
         <v>1826</v>
       </c>
+      <c r="F20" s="0" t="s">
+        <v>82</v>
+      </c>
       <c r="G20" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="I20" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2127,16 +2118,16 @@
       <c r="D21" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="E21" s="0" t="n">
+      <c r="E21" s="16" t="n">
         <v>1826</v>
       </c>
+      <c r="F21" s="0" t="s">
+        <v>82</v>
+      </c>
       <c r="G21" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="I21" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2153,16 +2144,16 @@
       <c r="D22" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="E22" s="0" t="n">
+      <c r="E22" s="16" t="n">
         <v>1826</v>
       </c>
+      <c r="F22" s="0" t="s">
+        <v>82</v>
+      </c>
       <c r="G22" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="I22" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2179,16 +2170,16 @@
       <c r="D23" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="E23" s="0" t="n">
+      <c r="E23" s="16" t="n">
         <v>1826</v>
       </c>
+      <c r="F23" s="0" t="s">
+        <v>82</v>
+      </c>
       <c r="G23" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="I23" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2205,16 +2196,16 @@
       <c r="D24" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="E24" s="0" t="n">
+      <c r="E24" s="16" t="n">
         <v>1826</v>
       </c>
+      <c r="F24" s="0" t="s">
+        <v>82</v>
+      </c>
       <c r="G24" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="I24" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2231,16 +2222,16 @@
       <c r="D25" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E25" s="0" t="n">
+      <c r="E25" s="16" t="n">
         <v>1844</v>
       </c>
+      <c r="F25" s="0" t="s">
+        <v>83</v>
+      </c>
       <c r="G25" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="I25" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2257,16 +2248,16 @@
       <c r="D26" s="16" t="n">
         <v>2.4</v>
       </c>
-      <c r="E26" s="0" t="n">
+      <c r="E26" s="16" t="n">
         <v>1832</v>
       </c>
+      <c r="F26" s="0" t="s">
+        <v>85</v>
+      </c>
       <c r="G26" s="0" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="I26" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2283,16 +2274,16 @@
       <c r="D27" s="16" t="n">
         <v>2.4</v>
       </c>
-      <c r="E27" s="0" t="n">
+      <c r="E27" s="16" t="n">
         <v>1832</v>
       </c>
+      <c r="F27" s="0" t="s">
+        <v>85</v>
+      </c>
       <c r="G27" s="0" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="I27" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2309,16 +2300,16 @@
       <c r="D28" s="16" t="n">
         <v>2.4</v>
       </c>
-      <c r="E28" s="0" t="n">
+      <c r="E28" s="16" t="n">
         <v>1832</v>
       </c>
+      <c r="F28" s="0" t="s">
+        <v>85</v>
+      </c>
       <c r="G28" s="0" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="I28" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2335,16 +2326,16 @@
       <c r="D29" s="16" t="n">
         <v>2.4</v>
       </c>
-      <c r="E29" s="0" t="n">
+      <c r="E29" s="16" t="n">
         <v>1832</v>
       </c>
+      <c r="F29" s="0" t="s">
+        <v>85</v>
+      </c>
       <c r="G29" s="0" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="I29" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2361,16 +2352,16 @@
       <c r="D30" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="E30" s="0" t="n">
+      <c r="E30" s="16" t="n">
         <v>1836</v>
       </c>
+      <c r="F30" s="0" t="s">
+        <v>86</v>
+      </c>
       <c r="G30" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="I30" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2387,16 +2378,16 @@
       <c r="D31" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="E31" s="0" t="n">
+      <c r="E31" s="16" t="n">
         <v>1836</v>
       </c>
+      <c r="F31" s="0" t="s">
+        <v>86</v>
+      </c>
       <c r="G31" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="I31" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2413,16 +2404,16 @@
       <c r="D32" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="E32" s="0" t="n">
+      <c r="E32" s="16" t="n">
         <v>1836</v>
       </c>
+      <c r="F32" s="0" t="s">
+        <v>86</v>
+      </c>
       <c r="G32" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="I32" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2439,16 +2430,16 @@
       <c r="D33" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E33" s="0" t="n">
+      <c r="E33" s="16" t="n">
         <v>1830</v>
       </c>
+      <c r="F33" s="0" t="s">
+        <v>89</v>
+      </c>
       <c r="G33" s="0" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="I33" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2465,16 +2456,16 @@
       <c r="D34" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="E34" s="0" t="n">
+      <c r="E34" s="16" t="n">
         <v>1830</v>
       </c>
+      <c r="F34" s="0" t="s">
+        <v>89</v>
+      </c>
       <c r="G34" s="0" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="I34" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2491,16 +2482,16 @@
       <c r="D35" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E35" s="0" t="n">
+      <c r="E35" s="16" t="n">
         <v>1827</v>
       </c>
+      <c r="F35" s="0" t="s">
+        <v>90</v>
+      </c>
       <c r="G35" s="0" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="I35" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2517,16 +2508,16 @@
       <c r="D36" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="E36" s="0" t="n">
+      <c r="E36" s="16" t="n">
         <v>1827</v>
       </c>
+      <c r="F36" s="0" t="s">
+        <v>90</v>
+      </c>
       <c r="G36" s="0" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="I36" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2543,16 +2534,16 @@
       <c r="D37" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="E37" s="0" t="n">
+      <c r="E37" s="16" t="n">
         <v>1827</v>
       </c>
+      <c r="F37" s="0" t="s">
+        <v>90</v>
+      </c>
       <c r="G37" s="0" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="I37" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2569,16 +2560,16 @@
       <c r="D38" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="E38" s="0" t="n">
+      <c r="E38" s="16" t="n">
         <v>1827</v>
       </c>
+      <c r="F38" s="0" t="s">
+        <v>90</v>
+      </c>
       <c r="G38" s="0" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="I38" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2595,16 +2586,16 @@
       <c r="D39" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="E39" s="0" t="n">
+      <c r="E39" s="16" t="n">
         <v>1827</v>
       </c>
+      <c r="F39" s="0" t="s">
+        <v>90</v>
+      </c>
       <c r="G39" s="0" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="I39" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2621,16 +2612,16 @@
       <c r="D40" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="E40" s="0" t="n">
+      <c r="E40" s="16" t="n">
         <v>1827</v>
       </c>
+      <c r="F40" s="0" t="s">
+        <v>90</v>
+      </c>
       <c r="G40" s="0" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="I40" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2647,16 +2638,16 @@
       <c r="D41" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="E41" s="0" t="n">
+      <c r="E41" s="16" t="n">
         <v>1827</v>
       </c>
+      <c r="F41" s="0" t="s">
+        <v>90</v>
+      </c>
       <c r="G41" s="0" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="I41" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2673,16 +2664,16 @@
       <c r="D42" s="16" t="n">
         <v>2.4</v>
       </c>
-      <c r="E42" s="0" t="n">
+      <c r="E42" s="16" t="n">
         <v>2833</v>
       </c>
+      <c r="F42" s="0" t="s">
+        <v>92</v>
+      </c>
       <c r="G42" s="0" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="I42" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2699,16 +2690,16 @@
       <c r="D43" s="16" t="n">
         <v>2.4</v>
       </c>
-      <c r="E43" s="0" t="n">
+      <c r="E43" s="16" t="n">
         <v>2833</v>
       </c>
+      <c r="F43" s="0" t="s">
+        <v>92</v>
+      </c>
       <c r="G43" s="0" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="I43" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2725,16 +2716,16 @@
       <c r="D44" s="16" t="n">
         <v>2.4</v>
       </c>
-      <c r="E44" s="0" t="n">
+      <c r="E44" s="16" t="n">
         <v>2833</v>
       </c>
+      <c r="F44" s="0" t="s">
+        <v>92</v>
+      </c>
       <c r="G44" s="0" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="I44" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2751,16 +2742,16 @@
       <c r="D45" s="16" t="n">
         <v>2.4</v>
       </c>
-      <c r="E45" s="0" t="n">
+      <c r="E45" s="16" t="n">
         <v>2833</v>
       </c>
+      <c r="F45" s="0" t="s">
+        <v>92</v>
+      </c>
       <c r="G45" s="0" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="I45" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2777,16 +2768,16 @@
       <c r="D46" s="16" t="n">
         <v>2.4</v>
       </c>
-      <c r="E46" s="0" t="n">
+      <c r="E46" s="16" t="n">
         <v>3833</v>
       </c>
+      <c r="F46" s="0" t="s">
+        <v>93</v>
+      </c>
       <c r="G46" s="0" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="I46" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2803,16 +2794,16 @@
       <c r="D47" s="16" t="n">
         <v>2.4</v>
       </c>
-      <c r="E47" s="0" t="n">
+      <c r="E47" s="16" t="n">
         <v>3833</v>
       </c>
+      <c r="F47" s="0" t="s">
+        <v>93</v>
+      </c>
       <c r="G47" s="0" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="I47" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2829,16 +2820,16 @@
       <c r="D48" s="16" t="n">
         <v>2.4</v>
       </c>
-      <c r="E48" s="0" t="n">
+      <c r="E48" s="16" t="n">
         <v>3833</v>
       </c>
+      <c r="F48" s="0" t="s">
+        <v>93</v>
+      </c>
       <c r="G48" s="0" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="I48" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2855,16 +2846,16 @@
       <c r="D49" s="16" t="n">
         <v>2.4</v>
       </c>
-      <c r="E49" s="0" t="n">
+      <c r="E49" s="16" t="n">
         <v>3833</v>
       </c>
+      <c r="F49" s="0" t="s">
+        <v>93</v>
+      </c>
       <c r="G49" s="0" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="I49" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2881,16 +2872,16 @@
       <c r="D50" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E50" s="0" t="n">
+      <c r="E50" s="16" t="n">
         <v>3835</v>
       </c>
+      <c r="F50" s="0" t="s">
+        <v>94</v>
+      </c>
       <c r="G50" s="0" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="I50" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2907,16 +2898,16 @@
       <c r="D51" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E51" s="0" t="n">
+      <c r="E51" s="16" t="n">
         <v>2835</v>
       </c>
+      <c r="F51" s="0" t="s">
+        <v>95</v>
+      </c>
       <c r="G51" s="0" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="I51" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2933,16 +2924,16 @@
       <c r="D52" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E52" s="0" t="n">
+      <c r="E52" s="16" t="n">
         <v>3833</v>
       </c>
+      <c r="F52" s="0" t="s">
+        <v>93</v>
+      </c>
       <c r="G52" s="0" t="s">
-        <v>93</v>
+        <v>63</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="I52" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2959,16 +2950,16 @@
       <c r="D53" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E53" s="0" t="n">
+      <c r="E53" s="16" t="n">
         <v>2833</v>
       </c>
+      <c r="F53" s="0" t="s">
+        <v>96</v>
+      </c>
       <c r="G53" s="0" t="s">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="I53" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2985,16 +2976,16 @@
       <c r="D54" s="16" t="n">
         <v>2.4</v>
       </c>
-      <c r="E54" s="0" t="n">
+      <c r="E54" s="16" t="n">
         <v>3833</v>
       </c>
+      <c r="F54" s="0" t="s">
+        <v>93</v>
+      </c>
       <c r="G54" s="0" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="I54" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3011,16 +3002,16 @@
       <c r="D55" s="16" t="n">
         <v>2.4</v>
       </c>
-      <c r="E55" s="0" t="n">
+      <c r="E55" s="16" t="n">
         <v>2833</v>
       </c>
+      <c r="F55" s="0" t="s">
+        <v>96</v>
+      </c>
       <c r="G55" s="0" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="I55" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3037,16 +3028,16 @@
       <c r="D56" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="E56" s="0" t="n">
+      <c r="E56" s="16" t="n">
         <v>3837</v>
       </c>
+      <c r="F56" s="0" t="s">
+        <v>97</v>
+      </c>
       <c r="G56" s="0" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="I56" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3063,16 +3054,16 @@
       <c r="D57" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="E57" s="0" t="n">
+      <c r="E57" s="16" t="n">
         <v>2837</v>
       </c>
+      <c r="F57" s="0" t="s">
+        <v>98</v>
+      </c>
       <c r="G57" s="0" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="H57" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="I57" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3089,16 +3080,16 @@
       <c r="D58" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="E58" s="0" t="n">
+      <c r="E58" s="16" t="n">
         <v>3837</v>
       </c>
+      <c r="F58" s="0" t="s">
+        <v>97</v>
+      </c>
       <c r="G58" s="0" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="H58" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="I58" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3115,16 +3106,16 @@
       <c r="D59" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="E59" s="0" t="n">
+      <c r="E59" s="16" t="n">
         <v>2837</v>
       </c>
+      <c r="F59" s="0" t="s">
+        <v>98</v>
+      </c>
       <c r="G59" s="0" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="H59" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="I59" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3141,16 +3132,16 @@
       <c r="D60" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="E60" s="0" t="n">
+      <c r="E60" s="16" t="n">
         <v>3837</v>
       </c>
+      <c r="F60" s="0" t="s">
+        <v>97</v>
+      </c>
       <c r="G60" s="0" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="H60" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="I60" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3167,16 +3158,16 @@
       <c r="D61" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="E61" s="0" t="n">
+      <c r="E61" s="16" t="n">
         <v>2837</v>
       </c>
+      <c r="F61" s="0" t="s">
+        <v>98</v>
+      </c>
       <c r="G61" s="0" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="H61" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="I61" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3193,16 +3184,16 @@
       <c r="D62" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E62" s="0" t="n">
+      <c r="E62" s="16" t="n">
         <v>3837</v>
       </c>
+      <c r="F62" s="0" t="s">
+        <v>99</v>
+      </c>
       <c r="G62" s="0" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="H62" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="I62" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3219,16 +3210,16 @@
       <c r="D63" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E63" s="0" t="n">
+      <c r="E63" s="16" t="n">
         <v>2837</v>
       </c>
+      <c r="F63" s="0" t="s">
+        <v>100</v>
+      </c>
       <c r="G63" s="0" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="H63" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="I63" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3245,16 +3236,16 @@
       <c r="D64" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="E64" s="0" t="n">
+      <c r="E64" s="16" t="n">
         <v>3837</v>
       </c>
+      <c r="F64" s="0" t="s">
+        <v>101</v>
+      </c>
       <c r="G64" s="0" t="s">
-        <v>101</v>
+        <v>69</v>
       </c>
       <c r="H64" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="I64" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3271,16 +3262,16 @@
       <c r="D65" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="E65" s="0" t="n">
+      <c r="E65" s="16" t="n">
         <v>2837</v>
       </c>
+      <c r="F65" s="0" t="s">
+        <v>100</v>
+      </c>
       <c r="G65" s="0" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="H65" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="I65" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3297,16 +3288,16 @@
       <c r="D66" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E66" s="0" t="n">
+      <c r="E66" s="16" t="n">
         <v>3839</v>
       </c>
+      <c r="F66" s="0" t="s">
+        <v>102</v>
+      </c>
       <c r="G66" s="0" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="H66" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="I66" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3323,16 +3314,16 @@
       <c r="D67" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E67" s="0" t="n">
+      <c r="E67" s="16" t="n">
         <v>2839</v>
       </c>
+      <c r="F67" s="0" t="s">
+        <v>103</v>
+      </c>
       <c r="G67" s="0" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="H67" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="I67" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3349,16 +3340,16 @@
       <c r="D68" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="E68" s="0" t="n">
+      <c r="E68" s="16" t="n">
         <v>3839</v>
       </c>
+      <c r="F68" s="0" t="s">
+        <v>102</v>
+      </c>
       <c r="G68" s="0" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="H68" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="I68" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3375,16 +3366,16 @@
       <c r="D69" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="E69" s="0" t="n">
+      <c r="E69" s="16" t="n">
         <v>2839</v>
       </c>
+      <c r="F69" s="0" t="s">
+        <v>103</v>
+      </c>
       <c r="G69" s="0" t="s">
-        <v>103</v>
+        <v>72</v>
       </c>
       <c r="H69" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="I69" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3401,16 +3392,16 @@
       <c r="D70" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="E70" s="0" t="n">
+      <c r="E70" s="16" t="n">
         <v>3839</v>
       </c>
+      <c r="F70" s="0" t="s">
+        <v>102</v>
+      </c>
       <c r="G70" s="0" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="H70" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="I70" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3427,16 +3418,16 @@
       <c r="D71" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="E71" s="0" t="n">
+      <c r="E71" s="16" t="n">
         <v>2839</v>
       </c>
+      <c r="F71" s="0" t="s">
+        <v>103</v>
+      </c>
       <c r="G71" s="0" t="s">
-        <v>103</v>
+        <v>72</v>
       </c>
       <c r="H71" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="I71" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3453,16 +3444,16 @@
       <c r="D72" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="E72" s="0" t="n">
+      <c r="E72" s="16" t="n">
         <v>3839</v>
       </c>
+      <c r="F72" s="0" t="s">
+        <v>104</v>
+      </c>
       <c r="G72" s="0" t="s">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="H72" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="I72" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3479,16 +3470,16 @@
       <c r="D73" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="E73" s="0" t="n">
+      <c r="E73" s="16" t="n">
         <v>2839</v>
       </c>
+      <c r="F73" s="0" t="s">
+        <v>103</v>
+      </c>
       <c r="G73" s="0" t="s">
-        <v>103</v>
+        <v>72</v>
       </c>
       <c r="H73" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="I73" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3505,16 +3496,16 @@
       <c r="D74" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="E74" s="0" t="n">
+      <c r="E74" s="16" t="n">
         <v>3841</v>
       </c>
+      <c r="F74" s="0" t="s">
+        <v>105</v>
+      </c>
       <c r="G74" s="0" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="H74" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="I74" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3531,16 +3522,16 @@
       <c r="D75" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="E75" s="0" t="n">
+      <c r="E75" s="16" t="n">
         <v>2841</v>
       </c>
+      <c r="F75" s="0" t="s">
+        <v>106</v>
+      </c>
       <c r="G75" s="0" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
       <c r="H75" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="I75" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3557,16 +3548,16 @@
       <c r="D76" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E76" s="0" t="n">
+      <c r="E76" s="16" t="n">
         <v>3841</v>
       </c>
+      <c r="F76" s="0" t="s">
+        <v>105</v>
+      </c>
       <c r="G76" s="0" t="s">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="H76" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="I76" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3583,16 +3574,16 @@
       <c r="D77" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E77" s="0" t="n">
+      <c r="E77" s="16" t="n">
         <v>2841</v>
       </c>
+      <c r="F77" s="0" t="s">
+        <v>106</v>
+      </c>
       <c r="G77" s="0" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="H77" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="I77" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3609,16 +3600,16 @@
       <c r="D78" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="E78" s="0" t="n">
+      <c r="E78" s="16" t="n">
         <v>3841</v>
       </c>
+      <c r="F78" s="0" t="s">
+        <v>105</v>
+      </c>
       <c r="G78" s="0" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="H78" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="I78" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3635,16 +3626,16 @@
       <c r="D79" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="E79" s="0" t="n">
+      <c r="E79" s="16" t="n">
         <v>2841</v>
       </c>
+      <c r="F79" s="0" t="s">
+        <v>106</v>
+      </c>
       <c r="G79" s="0" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
       <c r="H79" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="I79" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3661,16 +3652,16 @@
       <c r="D80" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E80" s="0" t="n">
+      <c r="E80" s="16" t="n">
         <v>3843</v>
       </c>
+      <c r="F80" s="0" t="s">
+        <v>107</v>
+      </c>
       <c r="G80" s="0" t="s">
-        <v>107</v>
+        <v>77</v>
       </c>
       <c r="H80" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="I80" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3687,16 +3678,16 @@
       <c r="D81" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E81" s="0" t="n">
+      <c r="E81" s="16" t="n">
         <v>2843</v>
       </c>
+      <c r="F81" s="0" t="s">
+        <v>108</v>
+      </c>
       <c r="G81" s="0" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="H81" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="I81" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3713,16 +3704,16 @@
       <c r="D82" s="16" t="n">
         <v>7</v>
       </c>
-      <c r="E82" s="0" t="n">
+      <c r="E82" s="16" t="n">
         <v>3843</v>
       </c>
+      <c r="F82" s="0" t="s">
+        <v>109</v>
+      </c>
       <c r="G82" s="0" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="H82" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="I82" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3739,16 +3730,16 @@
       <c r="D83" s="16" t="n">
         <v>7</v>
       </c>
-      <c r="E83" s="0" t="n">
+      <c r="E83" s="16" t="n">
         <v>2843</v>
       </c>
+      <c r="F83" s="0" t="s">
+        <v>108</v>
+      </c>
       <c r="G83" s="0" t="s">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="H83" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="I83" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3765,16 +3756,16 @@
       <c r="D84" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E84" s="0" t="n">
+      <c r="E84" s="16" t="n">
         <v>3845</v>
       </c>
+      <c r="F84" s="0" t="s">
+        <v>110</v>
+      </c>
       <c r="G84" s="0" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
       <c r="H84" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="I84" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3791,16 +3782,16 @@
       <c r="D85" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E85" s="0" t="n">
+      <c r="E85" s="16" t="n">
         <v>2845</v>
       </c>
+      <c r="F85" s="0" t="s">
+        <v>111</v>
+      </c>
       <c r="G85" s="0" t="s">
-        <v>111</v>
+        <v>84</v>
       </c>
       <c r="H85" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="I85" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3817,16 +3808,16 @@
       <c r="D86" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E86" s="0" t="n">
+      <c r="E86" s="16" t="n">
         <v>1831</v>
       </c>
+      <c r="F86" s="0" t="s">
+        <v>112</v>
+      </c>
       <c r="G86" s="0" t="s">
-        <v>112</v>
+        <v>80</v>
       </c>
       <c r="H86" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="I86" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3843,16 +3834,16 @@
       <c r="D87" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="E87" s="0" t="n">
+      <c r="E87" s="16" t="n">
         <v>1831</v>
       </c>
+      <c r="F87" s="0" t="s">
+        <v>112</v>
+      </c>
       <c r="G87" s="0" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="H87" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="I87" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3869,16 +3860,16 @@
       <c r="D88" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E88" s="0" t="n">
+      <c r="E88" s="16" t="n">
         <v>1828</v>
       </c>
+      <c r="F88" s="0" t="s">
+        <v>113</v>
+      </c>
       <c r="G88" s="0" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
       <c r="H88" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="I88" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3895,16 +3886,16 @@
       <c r="D89" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="E89" s="0" t="n">
+      <c r="E89" s="16" t="n">
         <v>1828</v>
       </c>
+      <c r="F89" s="0" t="s">
+        <v>113</v>
+      </c>
       <c r="G89" s="0" t="s">
-        <v>113</v>
+        <v>81</v>
       </c>
       <c r="H89" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="I89" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3921,16 +3912,16 @@
       <c r="D90" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="E90" s="0" t="n">
+      <c r="E90" s="16" t="n">
         <v>1828</v>
       </c>
+      <c r="F90" s="0" t="s">
+        <v>113</v>
+      </c>
       <c r="G90" s="0" t="s">
-        <v>113</v>
+        <v>81</v>
       </c>
       <c r="H90" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="I90" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3947,16 +3938,16 @@
       <c r="D91" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="E91" s="0" t="n">
+      <c r="E91" s="16" t="n">
         <v>1828</v>
       </c>
+      <c r="F91" s="0" t="s">
+        <v>113</v>
+      </c>
       <c r="G91" s="0" t="s">
-        <v>113</v>
+        <v>81</v>
       </c>
       <c r="H91" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="I91" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3973,16 +3964,16 @@
       <c r="D92" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="E92" s="0" t="n">
+      <c r="E92" s="16" t="n">
         <v>1828</v>
       </c>
+      <c r="F92" s="0" t="s">
+        <v>113</v>
+      </c>
       <c r="G92" s="0" t="s">
-        <v>113</v>
+        <v>81</v>
       </c>
       <c r="H92" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="I92" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3999,16 +3990,16 @@
       <c r="D93" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="E93" s="0" t="n">
+      <c r="E93" s="16" t="n">
         <v>1828</v>
       </c>
+      <c r="F93" s="0" t="s">
+        <v>113</v>
+      </c>
       <c r="G93" s="0" t="s">
-        <v>113</v>
+        <v>81</v>
       </c>
       <c r="H93" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="I93" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -4025,16 +4016,16 @@
       <c r="D94" s="16" t="n">
         <v>1.6</v>
       </c>
-      <c r="E94" s="0" t="n">
+      <c r="E94" s="16" t="n">
         <v>1828</v>
       </c>
+      <c r="F94" s="0" t="s">
+        <v>113</v>
+      </c>
       <c r="G94" s="0" t="s">
-        <v>113</v>
+        <v>81</v>
       </c>
       <c r="H94" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="I94" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -4062,9 +4053,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.7368421052632"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.8461538461538"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.0242914979757"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="64.2712550607287"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.3805668016194"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.3481781376518"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -4136,9 +4127,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.7368421052632"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.8461538461538"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.6599190283401"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="64.2712550607287"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.3805668016194"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="87.4089068825911"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -4210,9 +4201,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.7368421052632"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.8461538461538"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.0526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="64.2712550607287"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.3805668016194"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.6963562753036"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -4284,8 +4275,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="40.17004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="178.352226720648"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="40.5991902834008"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="179.95951417004"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="5" width="9.4251012145749"/>
   </cols>
   <sheetData>
@@ -4345,8 +4336,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="51.8461538461539"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="34.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="52.2753036437247"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="34.919028340081"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="5" width="9.4251012145749"/>
   </cols>
   <sheetData>
@@ -4406,9 +4397,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="64.7004048582996"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.8097165991903"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.5627530364373"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.2348178137652"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="59.2348178137652"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.8825910931174"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -4480,8 +4471,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="40.919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="126.878542510121"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="41.2388663967611"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="128.008097165992"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="5" width="9.4251012145749"/>
   </cols>
   <sheetData>
@@ -4541,8 +4532,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="52.7044534412956"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="81.4089068825911"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="53.1295546558704"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="82.1619433198381"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="5" width="9.4251012145749"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
marsru - small fix in the template
</commit_message>
<xml_diff>
--- a/Projects/MARSRU_PROD/Data/MARS must-range targets.xlsx
+++ b/Projects/MARSRU_PROD/Data/MARS must-range targets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="2217" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="93">
   <si>
     <t xml:space="preserve">KPI name</t>
   </si>
@@ -167,34 +167,6 @@
 4607065372156,
 4607065003944,
 4607065002688</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4607065003999,
-4607065004019,
-4607065004057,
-4607065004118,
-4607065375966,
-4607065376000,
-4607065376062,
-4607065372057,
-5000159373111,
-5000159438698,
-4011100157361,
-4607065003838,
-4607065374792,
-5000159438674,
-4607065374877,
-5000159451802,
-4607065378424,
-5000159425513,
-5000159438926,
-5000159438940,
-4607065371166,
-4607065372217,
-4607065372156,
-4607065003944,
-4607065002541
-</t>
   </si>
   <si>
     <t xml:space="preserve">4607065003999,
@@ -680,17 +652,17 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="1023" min="4" style="1" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="30.2348178137652"/>
+    <col collapsed="false" hidden="false" max="1023" min="4" style="1" width="9.66801619433198"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="9.66801619433198"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -716,7 +688,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="40.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="38.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
         <v>2310</v>
       </c>
@@ -751,10 +723,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.30364372469636"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="30.2348178137652"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.66801619433198"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -827,11 +799,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.2388663967611"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.2105263157895"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4251012145749"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.6396761133603"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.0971659919028"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.66801619433198"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -950,17 +922,17 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.0971659919028"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.1740890688259"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4251012145749"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.6153846153846"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.3805668016194"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.66801619433198"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1019,7 +991,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="350.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="321.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -1044,10 +1016,10 @@
         <v>13</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="336.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="321.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
@@ -1058,7 +1030,7 @@
         <v>13</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1085,89 +1057,89 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.2064777327935"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.3198380566802"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.2348178137652"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.4251012145749"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1194,102 +1166,102 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.3117408906883"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="30.3157894736842"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="28.0647773279352"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="10" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.9919028340081"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.7813765182186"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.919028340081"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.1336032388664"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="31.82995951417"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="29.3805668016194"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="10" width="18.7327935222672"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.1336032388664"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.587044534413"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.0364372469636"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.66801619433198"/>
   </cols>
   <sheetData>
     <row r="1" s="10" customFormat="true" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>38</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>39</v>
       </c>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="10" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>40</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="10" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>41</v>
       </c>
       <c r="E2" s="10" t="n">
         <v>1834</v>
       </c>
       <c r="F2" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="0" t="s">
-        <v>43</v>
-      </c>
       <c r="H2" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="10" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>40</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="10" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>41</v>
       </c>
       <c r="E3" s="10" t="n">
         <v>1832</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="10" t="n">
         <v>1.6</v>
@@ -1301,47 +1273,47 @@
         <v>1832</v>
       </c>
       <c r="F4" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="0" t="s">
-        <v>46</v>
-      </c>
       <c r="H4" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="10" t="n">
         <v>2.4</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E5" s="10" t="n">
         <v>1836</v>
       </c>
       <c r="F5" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="0" t="s">
-        <v>48</v>
-      </c>
       <c r="H5" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="10" t="n">
         <v>2.4</v>
@@ -1353,47 +1325,47 @@
         <v>1836</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="10" t="n">
         <v>3</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E7" s="10" t="n">
         <v>1838</v>
       </c>
       <c r="F7" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="0" t="s">
-        <v>51</v>
-      </c>
       <c r="H7" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="10" t="n">
         <v>3</v>
@@ -1405,21 +1377,21 @@
         <v>1838</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="10" t="n">
         <v>3</v>
@@ -1431,21 +1403,21 @@
         <v>1838</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="10" t="n">
         <v>3</v>
@@ -1457,21 +1429,21 @@
         <v>1838</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="10" t="n">
         <v>4</v>
@@ -1483,47 +1455,47 @@
         <v>1840</v>
       </c>
       <c r="F11" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="G11" s="0" t="s">
-        <v>54</v>
-      </c>
       <c r="H11" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" s="10" t="n">
         <v>4</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E12" s="10" t="n">
         <v>1840</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="10" t="n">
         <v>4</v>
@@ -1535,47 +1507,47 @@
         <v>1840</v>
       </c>
       <c r="F13" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="G13" s="0" t="s">
-        <v>54</v>
-      </c>
       <c r="H13" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" s="10" t="n">
         <v>5</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E14" s="10" t="n">
         <v>1842</v>
       </c>
       <c r="F14" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="G14" s="0" t="s">
-        <v>57</v>
-      </c>
       <c r="H14" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="10" t="n">
         <v>5</v>
@@ -1587,47 +1559,47 @@
         <v>1842</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>41</v>
-      </c>
       <c r="D16" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E16" s="10" t="n">
         <v>1829</v>
       </c>
       <c r="F16" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="G16" s="0" t="s">
-        <v>60</v>
-      </c>
       <c r="H16" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" s="10" t="n">
         <v>0</v>
@@ -1639,47 +1611,47 @@
         <v>1829</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>41</v>
-      </c>
       <c r="D18" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E18" s="10" t="n">
         <v>1826</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" s="10" t="n">
         <v>0</v>
@@ -1691,21 +1663,21 @@
         <v>1826</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" s="10" t="n">
         <v>0</v>
@@ -1717,21 +1689,21 @@
         <v>1826</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" s="10" t="n">
         <v>0</v>
@@ -1743,21 +1715,21 @@
         <v>1826</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" s="10" t="n">
         <v>0</v>
@@ -1769,21 +1741,21 @@
         <v>1826</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="10" t="n">
         <v>0</v>
@@ -1795,21 +1767,21 @@
         <v>1826</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24" s="10" t="n">
         <v>0</v>
@@ -1821,47 +1793,47 @@
         <v>1826</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C25" s="10" t="n">
         <v>7</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E25" s="10" t="n">
         <v>1844</v>
       </c>
       <c r="F25" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="G25" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="G25" s="0" t="s">
-        <v>64</v>
-      </c>
       <c r="H25" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C26" s="10" t="n">
         <v>1.6</v>
@@ -1873,21 +1845,21 @@
         <v>1832</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C27" s="10" t="n">
         <v>1.6</v>
@@ -1899,21 +1871,21 @@
         <v>1832</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C28" s="10" t="n">
         <v>1.6</v>
@@ -1925,21 +1897,21 @@
         <v>1832</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C29" s="10" t="n">
         <v>1.6</v>
@@ -1951,21 +1923,21 @@
         <v>1832</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C30" s="10" t="n">
         <v>2.4</v>
@@ -1977,21 +1949,21 @@
         <v>1836</v>
       </c>
       <c r="F30" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="G30" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="G30" s="0" t="s">
-        <v>67</v>
-      </c>
       <c r="H30" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C31" s="10" t="n">
         <v>2.4</v>
@@ -2003,21 +1975,21 @@
         <v>1836</v>
       </c>
       <c r="F31" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="G31" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="G31" s="0" t="s">
-        <v>67</v>
-      </c>
       <c r="H31" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C32" s="10" t="n">
         <v>2.4</v>
@@ -2029,47 +2001,47 @@
         <v>1836</v>
       </c>
       <c r="F32" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="G32" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="G32" s="0" t="s">
-        <v>67</v>
-      </c>
       <c r="H32" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E33" s="10" t="n">
         <v>1830</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C34" s="10" t="n">
         <v>0</v>
@@ -2081,47 +2053,47 @@
         <v>1830</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E35" s="10" t="n">
         <v>1827</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C36" s="10" t="n">
         <v>0</v>
@@ -2133,21 +2105,21 @@
         <v>1827</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C37" s="10" t="n">
         <v>0</v>
@@ -2159,21 +2131,21 @@
         <v>1827</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C38" s="10" t="n">
         <v>0</v>
@@ -2185,21 +2157,21 @@
         <v>1827</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C39" s="10" t="n">
         <v>0</v>
@@ -2211,21 +2183,21 @@
         <v>1827</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C40" s="10" t="n">
         <v>0</v>
@@ -2237,21 +2209,21 @@
         <v>1827</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C41" s="10" t="n">
         <v>0</v>
@@ -2263,21 +2235,21 @@
         <v>1827</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C42" s="10" t="n">
         <v>1.6</v>
@@ -2289,21 +2261,21 @@
         <v>2833</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C43" s="10" t="n">
         <v>1.6</v>
@@ -2315,21 +2287,21 @@
         <v>2833</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C44" s="10" t="n">
         <v>1.6</v>
@@ -2341,21 +2313,21 @@
         <v>2833</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C45" s="10" t="n">
         <v>1.6</v>
@@ -2367,21 +2339,21 @@
         <v>2833</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C46" s="10" t="n">
         <v>1.6</v>
@@ -2393,21 +2365,21 @@
         <v>3833</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C47" s="10" t="n">
         <v>1.6</v>
@@ -2419,21 +2391,21 @@
         <v>3833</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C48" s="10" t="n">
         <v>1.6</v>
@@ -2445,21 +2417,21 @@
         <v>3833</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C49" s="10" t="n">
         <v>1.6</v>
@@ -2471,125 +2443,125 @@
         <v>3833</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C50" s="10" t="n">
         <v>1.6</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E50" s="10" t="n">
         <v>3835</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C51" s="10" t="n">
         <v>1.6</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E51" s="10" t="n">
         <v>2835</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C52" s="10" t="n">
         <v>1.6</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E52" s="10" t="n">
         <v>3833</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C53" s="10" t="n">
         <v>1.6</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E53" s="10" t="n">
         <v>2833</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C54" s="10" t="n">
         <v>1.6</v>
@@ -2601,21 +2573,21 @@
         <v>3833</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C55" s="10" t="n">
         <v>1.6</v>
@@ -2627,21 +2599,21 @@
         <v>2833</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C56" s="10" t="n">
         <v>2.4</v>
@@ -2653,21 +2625,21 @@
         <v>3837</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C57" s="10" t="n">
         <v>2.4</v>
@@ -2679,21 +2651,21 @@
         <v>2837</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H57" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C58" s="10" t="n">
         <v>2.4</v>
@@ -2705,21 +2677,21 @@
         <v>3837</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H58" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C59" s="10" t="n">
         <v>2.4</v>
@@ -2731,21 +2703,21 @@
         <v>2837</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H59" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C60" s="10" t="n">
         <v>2.4</v>
@@ -2757,21 +2729,21 @@
         <v>3837</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H60" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C61" s="10" t="n">
         <v>2.4</v>
@@ -2783,73 +2755,73 @@
         <v>2837</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H61" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C62" s="10" t="n">
         <v>2.4</v>
       </c>
       <c r="D62" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E62" s="10" t="n">
         <v>3837</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G62" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H62" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C63" s="10" t="n">
         <v>2.4</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E63" s="10" t="n">
         <v>2837</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H63" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C64" s="10" t="n">
         <v>2.4</v>
@@ -2861,21 +2833,21 @@
         <v>3837</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G64" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H64" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C65" s="10" t="n">
         <v>2.4</v>
@@ -2887,73 +2859,73 @@
         <v>2837</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H65" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C66" s="10" t="n">
         <v>3</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E66" s="10" t="n">
         <v>3839</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H66" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C67" s="10" t="n">
         <v>3</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E67" s="10" t="n">
         <v>2839</v>
       </c>
       <c r="F67" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G67" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H67" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C68" s="10" t="n">
         <v>3</v>
@@ -2965,21 +2937,21 @@
         <v>3839</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G68" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H68" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C69" s="10" t="n">
         <v>3</v>
@@ -2991,21 +2963,21 @@
         <v>2839</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G69" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H69" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C70" s="10" t="n">
         <v>3</v>
@@ -3017,21 +2989,21 @@
         <v>3839</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G70" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H70" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C71" s="10" t="n">
         <v>3</v>
@@ -3043,21 +3015,21 @@
         <v>2839</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G71" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H71" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C72" s="10" t="n">
         <v>3</v>
@@ -3069,21 +3041,21 @@
         <v>3839</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G72" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H72" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C73" s="10" t="n">
         <v>3</v>
@@ -3095,21 +3067,21 @@
         <v>2839</v>
       </c>
       <c r="F73" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G73" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H73" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C74" s="10" t="n">
         <v>4</v>
@@ -3121,21 +3093,21 @@
         <v>3841</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G74" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H74" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C75" s="10" t="n">
         <v>4</v>
@@ -3147,73 +3119,73 @@
         <v>2841</v>
       </c>
       <c r="F75" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G75" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H75" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C76" s="10" t="n">
         <v>4</v>
       </c>
       <c r="D76" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E76" s="10" t="n">
         <v>3841</v>
       </c>
       <c r="F76" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G76" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H76" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C77" s="10" t="n">
         <v>4</v>
       </c>
       <c r="D77" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E77" s="10" t="n">
         <v>2841</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G77" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H77" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C78" s="10" t="n">
         <v>4</v>
@@ -3225,21 +3197,21 @@
         <v>3841</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G78" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H78" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C79" s="10" t="n">
         <v>4</v>
@@ -3251,73 +3223,73 @@
         <v>2841</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H79" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C80" s="10" t="n">
         <v>5</v>
       </c>
       <c r="D80" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E80" s="10" t="n">
         <v>3843</v>
       </c>
       <c r="F80" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G80" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H80" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C81" s="10" t="n">
         <v>5</v>
       </c>
       <c r="D81" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E81" s="10" t="n">
         <v>2843</v>
       </c>
       <c r="F81" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G81" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H81" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C82" s="10" t="n">
         <v>5</v>
@@ -3329,21 +3301,21 @@
         <v>3843</v>
       </c>
       <c r="F82" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G82" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H82" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C83" s="10" t="n">
         <v>5</v>
@@ -3355,99 +3327,99 @@
         <v>2843</v>
       </c>
       <c r="F83" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G83" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H83" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C84" s="10" t="n">
         <v>7</v>
       </c>
       <c r="D84" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E84" s="10" t="n">
         <v>3845</v>
       </c>
       <c r="F84" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G84" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H84" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C85" s="10" t="n">
         <v>7</v>
       </c>
       <c r="D85" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E85" s="10" t="n">
         <v>2845</v>
       </c>
       <c r="F85" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G85" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H85" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C86" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D86" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E86" s="10" t="n">
         <v>1831</v>
       </c>
       <c r="F86" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G86" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H86" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C87" s="10" t="n">
         <v>0</v>
@@ -3459,47 +3431,47 @@
         <v>1831</v>
       </c>
       <c r="F87" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G87" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H87" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C88" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D88" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E88" s="10" t="n">
         <v>1828</v>
       </c>
       <c r="F88" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G88" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H88" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C89" s="10" t="n">
         <v>0</v>
@@ -3511,21 +3483,21 @@
         <v>1828</v>
       </c>
       <c r="F89" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G89" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H89" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C90" s="10" t="n">
         <v>0</v>
@@ -3537,21 +3509,21 @@
         <v>1828</v>
       </c>
       <c r="F90" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G90" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H90" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C91" s="10" t="n">
         <v>0</v>
@@ -3563,21 +3535,21 @@
         <v>1828</v>
       </c>
       <c r="F91" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G91" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H91" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C92" s="10" t="n">
         <v>0</v>
@@ -3589,21 +3561,21 @@
         <v>1828</v>
       </c>
       <c r="F92" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G92" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H92" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C93" s="10" t="n">
         <v>0</v>
@@ -3615,21 +3587,21 @@
         <v>1828</v>
       </c>
       <c r="F93" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G93" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H93" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C94" s="10" t="n">
         <v>0</v>
@@ -3641,13 +3613,13 @@
         <v>1828</v>
       </c>
       <c r="F94" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G94" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H94" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MARSRU - template uploading hot fix
</commit_message>
<xml_diff>
--- a/Projects/MARSRU_PROD/Data/MARS must-range targets.xlsx
+++ b/Projects/MARSRU_PROD/Data/MARS must-range targets.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="99">
   <si>
     <t xml:space="preserve">Store type</t>
   </si>
@@ -45,33 +45,13 @@
 Grocery Магазин у дома (450-599),
 Grocery Магазин у дома (600-999),
 Grocery BIG BOXES (1000-2499),
-Grocery BIG BOXES (2500+)
-</t>
+Grocery BIG BOXES (2500+)</t>
   </si>
   <si>
     <t xml:space="preserve">4607065001063/5998749123072,
 4607065001025/5998749123058,
 4607065004514,
 4607065004446</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Grocery Магазин у дома (&lt;100),
-Grocery Магазин у дома (100-299),
-Grocery Магазин у дома (300-449),
-Grocery Магазин у дома (450-599),
-Grocery Магазин у дома (600-999),
-Grocery BIG BOXES (1000-2499),
-Grocery BIG BOXES (2500+)
-</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">5998749106877,
@@ -133,8 +113,7 @@
     <t xml:space="preserve">1+2 кластер,
 2-ой Food,
 2-ой Gr,
-2-ой ZOO
-</t>
+2-ой ZOO</t>
   </si>
   <si>
     <t xml:space="preserve">4607065376048,
@@ -147,8 +126,7 @@
     <t xml:space="preserve">3+4 кластер,
 3-ий Food,
 3-ий Gr,
-3-ий ZOO
-</t>
+3-ий ZOO</t>
   </si>
   <si>
     <t xml:space="preserve">4607065376048
@@ -173,11 +151,25 @@
 5000159438735</t>
   </si>
   <si>
+    <t xml:space="preserve">1+2 кластер,
+2-ой Food,
+2-ой Gr,
+2-ой ZOO
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">4607065376048,
 4607065002862,
 4607065377908,
 4607065375119,
 5000159450881</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3+4 кластер,
+3-ий Food,
+3-ий Gr,
+3-ий ZOO
+</t>
   </si>
   <si>
     <t xml:space="preserve">4607065376048,
@@ -468,7 +460,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -496,13 +488,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val=""/>
-      <family val="1"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -535,7 +520,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -563,10 +548,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -577,7 +558,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -585,7 +566,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -630,15 +611,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 4" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -711,16 +691,16 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.4412955465587"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.2834008097166"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.85425101214575"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="31.5627530364372"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="2" width="10.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="32.8502024291498"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.71255060728745"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="32.9919028340081"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="2" width="10.5708502024292"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -738,7 +718,7 @@
       </c>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" customFormat="false" ht="106" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="93" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -752,9 +732,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="107" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="93" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>2310</v>
@@ -763,12 +743,12 @@
         <v>1847</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="41" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3" t="n">
         <v>2310</v>
@@ -777,12 +757,12 @@
         <v>1846</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="3" t="n">
         <v>2310</v>
@@ -791,7 +771,7 @@
         <v>1847</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -813,16 +793,16 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.4412955465587"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="9.85425101214575"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="9.71255060728745"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="31.5627530364372"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="2" width="10.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="32.8502024291498"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="10.1417004048583"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="32.9919028340081"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="2" width="10.5708502024292"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -839,7 +819,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="106" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="93" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -853,9 +833,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="107" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="93" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>2330</v>
@@ -864,12 +844,12 @@
         <v>1849</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="41" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3" t="n">
         <v>2330</v>
@@ -878,12 +858,12 @@
         <v>1848</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="3" t="n">
         <v>2330</v>
@@ -892,7 +872,7 @@
         <v>1849</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -913,22 +893,22 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4251012145749"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.2834008097166"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.9878542510121"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.4251012145749"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.71255060728745"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.5587044534413"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.5708502024292"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>1</v>
@@ -942,69 +922,69 @@
     </row>
     <row r="2" customFormat="false" ht="275" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="6" t="n">
         <v>2254</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="275" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="6" t="n">
         <v>2254</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="275" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="6" t="n">
         <v>2254</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="80" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="6" t="n">
         <v>2254</v>
       </c>
       <c r="C5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>19</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="80" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B6" s="6" t="n">
         <v>2254</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>21</v>
@@ -1012,16 +992,16 @@
     </row>
     <row r="7" customFormat="false" ht="80" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B7" s="6" t="n">
         <v>2254</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1042,22 +1022,22 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="22.4251012145749"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="9.85425101214575"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="9" width="55.9878542510121"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="9" width="30.7085020242915"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="9" width="10.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="23.4251012145749"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="9" width="58.5587044534413"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="9" width="32.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="9" width="10.5708502024292"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>1</v>
@@ -1071,86 +1051,86 @@
     </row>
     <row r="2" customFormat="false" ht="327" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="6" t="n">
         <v>2254</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="327" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="6" t="n">
         <v>2254</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="327" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="6" t="n">
         <v>2254</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="327" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="6" t="n">
         <v>2254</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="327" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="6" t="n">
         <v>2254</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="327" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="6" t="n">
         <v>2254</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1177,9 +1157,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="46.2753036437247"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="31.5627530364372"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="9.85425101214575"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="48.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="32.9919028340081"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="10.2834008097166"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="34" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1187,79 +1167,79 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1286,102 +1266,102 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.5668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.9919028340081"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="33.2793522267206"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="12" width="30.7085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="19.5668016194332"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.2753036437247"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.4251012145749"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.2793522267206"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.2834008097166"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.9919028340081"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="34.7085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="12" width="32.1376518218623"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="20.4251012145749"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="51.5587044534413"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.2793522267206"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.5627530364372"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5708502024292"/>
   </cols>
   <sheetData>
     <row r="1" s="12" customFormat="true" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" s="12" t="n">
         <v>1.6</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E2" s="12" t="n">
         <v>1834</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C3" s="12" t="n">
         <v>1.6</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E3" s="12" t="n">
         <v>1832</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C4" s="12" t="n">
         <v>1.6</v>
@@ -1393,47 +1373,47 @@
         <v>1832</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C5" s="12" t="n">
         <v>2.4</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E5" s="12" t="n">
         <v>1836</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C6" s="12" t="n">
         <v>2.4</v>
@@ -1445,47 +1425,47 @@
         <v>1836</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C7" s="12" t="n">
         <v>3</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E7" s="12" t="n">
         <v>1838</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C8" s="12" t="n">
         <v>3</v>
@@ -1497,21 +1477,21 @@
         <v>1838</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9" s="12" t="n">
         <v>3</v>
@@ -1523,21 +1503,21 @@
         <v>1838</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C10" s="12" t="n">
         <v>3</v>
@@ -1549,21 +1529,21 @@
         <v>1838</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C11" s="12" t="n">
         <v>4</v>
@@ -1575,47 +1555,47 @@
         <v>1840</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C12" s="12" t="n">
         <v>4</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E12" s="12" t="n">
         <v>1840</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C13" s="12" t="n">
         <v>4</v>
@@ -1627,47 +1607,47 @@
         <v>1840</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C14" s="12" t="n">
         <v>5</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E14" s="12" t="n">
         <v>1842</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C15" s="12" t="n">
         <v>5</v>
@@ -1679,47 +1659,47 @@
         <v>1842</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E16" s="12" t="n">
         <v>1829</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C17" s="12" t="n">
         <v>0</v>
@@ -1731,47 +1711,47 @@
         <v>1829</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E18" s="12" t="n">
         <v>1826</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C19" s="12" t="n">
         <v>0</v>
@@ -1783,21 +1763,21 @@
         <v>1826</v>
       </c>
       <c r="F19" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="G19" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="G19" s="0" t="s">
-        <v>65</v>
-      </c>
       <c r="H19" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C20" s="12" t="n">
         <v>0</v>
@@ -1809,21 +1789,21 @@
         <v>1826</v>
       </c>
       <c r="F20" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="G20" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="G20" s="0" t="s">
-        <v>65</v>
-      </c>
       <c r="H20" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C21" s="12" t="n">
         <v>0</v>
@@ -1835,21 +1815,21 @@
         <v>1826</v>
       </c>
       <c r="F21" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="G21" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="G21" s="0" t="s">
-        <v>65</v>
-      </c>
       <c r="H21" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C22" s="12" t="n">
         <v>0</v>
@@ -1861,21 +1841,21 @@
         <v>1826</v>
       </c>
       <c r="F22" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="G22" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="G22" s="0" t="s">
-        <v>65</v>
-      </c>
       <c r="H22" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C23" s="12" t="n">
         <v>0</v>
@@ -1887,21 +1867,21 @@
         <v>1826</v>
       </c>
       <c r="F23" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="G23" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="G23" s="0" t="s">
-        <v>65</v>
-      </c>
       <c r="H23" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C24" s="12" t="n">
         <v>0</v>
@@ -1913,47 +1893,47 @@
         <v>1826</v>
       </c>
       <c r="F24" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="G24" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="G24" s="0" t="s">
-        <v>65</v>
-      </c>
       <c r="H24" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C25" s="12" t="n">
         <v>7</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E25" s="12" t="n">
         <v>1844</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C26" s="12" t="n">
         <v>1.6</v>
@@ -1965,21 +1945,21 @@
         <v>1832</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C27" s="12" t="n">
         <v>1.6</v>
@@ -1991,21 +1971,21 @@
         <v>1832</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C28" s="12" t="n">
         <v>1.6</v>
@@ -2017,21 +1997,21 @@
         <v>1832</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C29" s="12" t="n">
         <v>1.6</v>
@@ -2043,21 +2023,21 @@
         <v>1832</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C30" s="12" t="n">
         <v>2.4</v>
@@ -2069,21 +2049,21 @@
         <v>1836</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C31" s="12" t="n">
         <v>2.4</v>
@@ -2095,21 +2075,21 @@
         <v>1836</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C32" s="12" t="n">
         <v>2.4</v>
@@ -2121,47 +2101,47 @@
         <v>1836</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E33" s="12" t="n">
         <v>1830</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C34" s="12" t="n">
         <v>0</v>
@@ -2173,47 +2153,47 @@
         <v>1830</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E35" s="12" t="n">
         <v>1827</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C36" s="12" t="n">
         <v>0</v>
@@ -2225,21 +2205,21 @@
         <v>1827</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C37" s="12" t="n">
         <v>0</v>
@@ -2251,21 +2231,21 @@
         <v>1827</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C38" s="12" t="n">
         <v>0</v>
@@ -2277,21 +2257,21 @@
         <v>1827</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C39" s="12" t="n">
         <v>0</v>
@@ -2303,21 +2283,21 @@
         <v>1827</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C40" s="12" t="n">
         <v>0</v>
@@ -2329,21 +2309,21 @@
         <v>1827</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C41" s="12" t="n">
         <v>0</v>
@@ -2355,21 +2335,21 @@
         <v>1827</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C42" s="12" t="n">
         <v>1.6</v>
@@ -2381,21 +2361,21 @@
         <v>2833</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C43" s="12" t="n">
         <v>1.6</v>
@@ -2407,21 +2387,21 @@
         <v>2833</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C44" s="12" t="n">
         <v>1.6</v>
@@ -2433,21 +2413,21 @@
         <v>2833</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C45" s="12" t="n">
         <v>1.6</v>
@@ -2459,21 +2439,21 @@
         <v>2833</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C46" s="12" t="n">
         <v>1.6</v>
@@ -2485,21 +2465,21 @@
         <v>3833</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C47" s="12" t="n">
         <v>1.6</v>
@@ -2511,21 +2491,21 @@
         <v>3833</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C48" s="12" t="n">
         <v>1.6</v>
@@ -2537,21 +2517,21 @@
         <v>3833</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C49" s="12" t="n">
         <v>1.6</v>
@@ -2563,125 +2543,125 @@
         <v>3833</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C50" s="12" t="n">
         <v>1.6</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E50" s="12" t="n">
         <v>3835</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C51" s="12" t="n">
         <v>1.6</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E51" s="12" t="n">
         <v>2835</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C52" s="12" t="n">
         <v>1.6</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E52" s="12" t="n">
         <v>3833</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C53" s="12" t="n">
         <v>1.6</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E53" s="12" t="n">
         <v>2833</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C54" s="12" t="n">
         <v>1.6</v>
@@ -2693,21 +2673,21 @@
         <v>3833</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C55" s="12" t="n">
         <v>1.6</v>
@@ -2719,21 +2699,21 @@
         <v>2833</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C56" s="12" t="n">
         <v>2.4</v>
@@ -2745,21 +2725,21 @@
         <v>3837</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C57" s="12" t="n">
         <v>2.4</v>
@@ -2771,21 +2751,21 @@
         <v>2837</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H57" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C58" s="12" t="n">
         <v>2.4</v>
@@ -2797,21 +2777,21 @@
         <v>3837</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H58" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C59" s="12" t="n">
         <v>2.4</v>
@@ -2823,21 +2803,21 @@
         <v>2837</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H59" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C60" s="12" t="n">
         <v>2.4</v>
@@ -2849,21 +2829,21 @@
         <v>3837</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H60" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C61" s="12" t="n">
         <v>2.4</v>
@@ -2875,73 +2855,73 @@
         <v>2837</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H61" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C62" s="12" t="n">
         <v>2.4</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E62" s="12" t="n">
         <v>3837</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G62" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H62" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C63" s="12" t="n">
         <v>2.4</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E63" s="12" t="n">
         <v>2837</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H63" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C64" s="12" t="n">
         <v>2.4</v>
@@ -2953,21 +2933,21 @@
         <v>3837</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G64" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H64" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C65" s="12" t="n">
         <v>2.4</v>
@@ -2979,73 +2959,73 @@
         <v>2837</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H65" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C66" s="12" t="n">
         <v>3</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E66" s="12" t="n">
         <v>3839</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H66" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C67" s="12" t="n">
         <v>3</v>
       </c>
       <c r="D67" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E67" s="12" t="n">
         <v>2839</v>
       </c>
       <c r="F67" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G67" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H67" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C68" s="12" t="n">
         <v>3</v>
@@ -3057,21 +3037,21 @@
         <v>3839</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G68" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H68" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C69" s="12" t="n">
         <v>3</v>
@@ -3083,21 +3063,21 @@
         <v>2839</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G69" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H69" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C70" s="12" t="n">
         <v>3</v>
@@ -3109,21 +3089,21 @@
         <v>3839</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G70" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H70" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C71" s="12" t="n">
         <v>3</v>
@@ -3135,21 +3115,21 @@
         <v>2839</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G71" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H71" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C72" s="12" t="n">
         <v>3</v>
@@ -3161,21 +3141,21 @@
         <v>3839</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G72" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H72" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C73" s="12" t="n">
         <v>3</v>
@@ -3187,21 +3167,21 @@
         <v>2839</v>
       </c>
       <c r="F73" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G73" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H73" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C74" s="12" t="n">
         <v>4</v>
@@ -3213,21 +3193,21 @@
         <v>3841</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G74" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H74" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C75" s="12" t="n">
         <v>4</v>
@@ -3239,73 +3219,73 @@
         <v>2841</v>
       </c>
       <c r="F75" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G75" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H75" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C76" s="12" t="n">
         <v>4</v>
       </c>
       <c r="D76" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E76" s="12" t="n">
         <v>3841</v>
       </c>
       <c r="F76" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G76" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H76" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C77" s="12" t="n">
         <v>4</v>
       </c>
       <c r="D77" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E77" s="12" t="n">
         <v>2841</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G77" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H77" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C78" s="12" t="n">
         <v>4</v>
@@ -3317,21 +3297,21 @@
         <v>3841</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G78" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H78" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C79" s="12" t="n">
         <v>4</v>
@@ -3343,73 +3323,73 @@
         <v>2841</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H79" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C80" s="12" t="n">
         <v>5</v>
       </c>
       <c r="D80" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E80" s="12" t="n">
         <v>3843</v>
       </c>
       <c r="F80" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G80" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H80" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C81" s="12" t="n">
         <v>5</v>
       </c>
       <c r="D81" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E81" s="12" t="n">
         <v>2843</v>
       </c>
       <c r="F81" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G81" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H81" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C82" s="12" t="n">
         <v>5</v>
@@ -3421,21 +3401,21 @@
         <v>3843</v>
       </c>
       <c r="F82" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G82" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H82" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C83" s="12" t="n">
         <v>5</v>
@@ -3447,99 +3427,99 @@
         <v>2843</v>
       </c>
       <c r="F83" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G83" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H83" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C84" s="12" t="n">
         <v>7</v>
       </c>
       <c r="D84" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E84" s="12" t="n">
         <v>3845</v>
       </c>
       <c r="F84" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G84" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H84" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C85" s="12" t="n">
         <v>7</v>
       </c>
       <c r="D85" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E85" s="12" t="n">
         <v>2845</v>
       </c>
       <c r="F85" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G85" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H85" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C86" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D86" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E86" s="12" t="n">
         <v>1831</v>
       </c>
       <c r="F86" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G86" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H86" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C87" s="12" t="n">
         <v>0</v>
@@ -3551,47 +3531,47 @@
         <v>1831</v>
       </c>
       <c r="F87" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G87" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H87" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C88" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D88" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E88" s="12" t="n">
         <v>1828</v>
       </c>
       <c r="F88" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G88" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H88" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C89" s="12" t="n">
         <v>0</v>
@@ -3603,21 +3583,21 @@
         <v>1828</v>
       </c>
       <c r="F89" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G89" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H89" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C90" s="12" t="n">
         <v>0</v>
@@ -3629,21 +3609,21 @@
         <v>1828</v>
       </c>
       <c r="F90" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G90" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H90" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C91" s="12" t="n">
         <v>0</v>
@@ -3655,21 +3635,21 @@
         <v>1828</v>
       </c>
       <c r="F91" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G91" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H91" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C92" s="12" t="n">
         <v>0</v>
@@ -3681,21 +3661,21 @@
         <v>1828</v>
       </c>
       <c r="F92" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G92" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H92" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C93" s="12" t="n">
         <v>0</v>
@@ -3707,21 +3687,21 @@
         <v>1828</v>
       </c>
       <c r="F93" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G93" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H93" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C94" s="12" t="n">
         <v>0</v>
@@ -3733,13 +3713,13 @@
         <v>1828</v>
       </c>
       <c r="F94" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G94" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H94" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>